<commit_message>
changed the definition of expansion
</commit_message>
<xml_diff>
--- a/big_functions_frame.xlsx
+++ b/big_functions_frame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ssd980/teaching/gis_in_r/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ssd980/datasci_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F452D5-3AC0-C745-AAFF-6B97544AFC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED56A00-F477-3B4D-82A6-BC243C266571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{95C4795D-FAAA-484B-ACF2-0B904DFB98DD}"/>
+    <workbookView xWindow="21600" yWindow="0" windowWidth="68800" windowHeight="28800" xr2:uid="{95C4795D-FAAA-484B-ACF2-0B904DFB98DD}"/>
   </bookViews>
   <sheets>
     <sheet name="big_functions_frame" sheetId="1" r:id="rId1"/>
@@ -898,9 +898,6 @@
     <t>expansion</t>
   </si>
   <si>
-    <t>Set upper and lower values or proportions to expand an axis by</t>
-  </si>
-  <si>
     <t>facet_wrap</t>
   </si>
   <si>
@@ -2012,6 +2009,9 @@
   </si>
   <si>
     <t>Download and install one or more packages onto your computer</t>
+  </si>
+  <si>
+    <t>Set upper and lower values of a plot axis based on the range of data</t>
   </si>
 </sst>
 </file>
@@ -2874,8 +2874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26B7B1B-D76F-6446-A51A-BD765778C143}">
   <dimension ref="A1:D313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
-      <selection activeCell="D294" sqref="D294"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2907,7 +2907,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -2921,7 +2921,7 @@
         <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D3" t="s">
         <v>59</v>
@@ -2935,7 +2935,7 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -2949,7 +2949,7 @@
         <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D5" t="s">
         <v>156</v>
@@ -2963,7 +2963,7 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
@@ -2977,7 +2977,7 @@
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D7" t="s">
         <v>61</v>
@@ -2991,7 +2991,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -3005,7 +3005,7 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
@@ -3019,7 +3019,7 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -3030,10 +3030,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D11" t="s">
         <v>188</v>
@@ -3044,10 +3044,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D12" t="s">
         <v>189</v>
@@ -3061,7 +3061,7 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D13" t="s">
         <v>37</v>
@@ -3075,7 +3075,7 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -3089,7 +3089,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -3103,7 +3103,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -3117,7 +3117,7 @@
         <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D17" t="s">
         <v>158</v>
@@ -3131,7 +3131,7 @@
         <v>159</v>
       </c>
       <c r="C18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D18" t="s">
         <v>160</v>
@@ -3145,7 +3145,7 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
@@ -3159,7 +3159,7 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D20" t="s">
         <v>27</v>
@@ -3173,7 +3173,7 @@
         <v>161</v>
       </c>
       <c r="C21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D21" t="s">
         <v>163</v>
@@ -3187,7 +3187,7 @@
         <v>162</v>
       </c>
       <c r="C22" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D22" t="s">
         <v>164</v>
@@ -3201,7 +3201,7 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -3215,7 +3215,7 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
@@ -3229,7 +3229,7 @@
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -3243,7 +3243,7 @@
         <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
@@ -3257,7 +3257,7 @@
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D27" t="s">
         <v>19</v>
@@ -3271,7 +3271,7 @@
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D28" t="s">
         <v>39</v>
@@ -3285,7 +3285,7 @@
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D29" t="s">
         <v>41</v>
@@ -3299,7 +3299,7 @@
         <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D30" t="s">
         <v>43</v>
@@ -3313,7 +3313,7 @@
         <v>165</v>
       </c>
       <c r="C31" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D31" t="s">
         <v>166</v>
@@ -3327,7 +3327,7 @@
         <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D32" t="s">
         <v>45</v>
@@ -3338,13 +3338,13 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C33" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D33" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3355,7 +3355,7 @@
         <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D34" t="s">
         <v>47</v>
@@ -3369,7 +3369,7 @@
         <v>167</v>
       </c>
       <c r="C35" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D35" t="s">
         <v>168</v>
@@ -3383,7 +3383,7 @@
         <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D36" t="s">
         <v>49</v>
@@ -3397,7 +3397,7 @@
         <v>182</v>
       </c>
       <c r="C37" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D37" t="s">
         <v>183</v>
@@ -3411,10 +3411,10 @@
         <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D38" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -3425,7 +3425,7 @@
         <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D39" t="s">
         <v>51</v>
@@ -3439,7 +3439,7 @@
         <v>169</v>
       </c>
       <c r="C40" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D40" t="s">
         <v>170</v>
@@ -3453,7 +3453,7 @@
         <v>172</v>
       </c>
       <c r="C41" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D41" t="s">
         <v>171</v>
@@ -3467,7 +3467,7 @@
         <v>173</v>
       </c>
       <c r="C42" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D42" t="s">
         <v>174</v>
@@ -3481,7 +3481,7 @@
         <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D43" t="s">
         <v>53</v>
@@ -3495,7 +3495,7 @@
         <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D44" t="s">
         <v>55</v>
@@ -3509,7 +3509,7 @@
         <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D45" t="s">
         <v>57</v>
@@ -3523,7 +3523,7 @@
         <v>175</v>
       </c>
       <c r="C46" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D46" t="s">
         <v>176</v>
@@ -3537,7 +3537,7 @@
         <v>58</v>
       </c>
       <c r="C47" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D47" t="s">
         <v>177</v>
@@ -3551,7 +3551,7 @@
         <v>178</v>
       </c>
       <c r="C48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D48" t="s">
         <v>179</v>
@@ -3565,7 +3565,7 @@
         <v>181</v>
       </c>
       <c r="C49" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D49" t="s">
         <v>180</v>
@@ -3576,13 +3576,13 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
+        <v>489</v>
+      </c>
+      <c r="C50" t="s">
+        <v>418</v>
+      </c>
+      <c r="D50" t="s">
         <v>490</v>
-      </c>
-      <c r="C50" t="s">
-        <v>419</v>
-      </c>
-      <c r="D50" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -3593,7 +3593,7 @@
         <v>184</v>
       </c>
       <c r="C51" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D51" t="s">
         <v>185</v>
@@ -3601,16 +3601,16 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>617</v>
+      </c>
+      <c r="B52" t="s">
         <v>618</v>
       </c>
-      <c r="B52" t="s">
-        <v>619</v>
-      </c>
       <c r="C52" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D52" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -3621,7 +3621,7 @@
         <v>186</v>
       </c>
       <c r="C53" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D53" t="s">
         <v>187</v>
@@ -3632,13 +3632,13 @@
         <v>62</v>
       </c>
       <c r="B54" t="s">
+        <v>449</v>
+      </c>
+      <c r="C54" t="s">
+        <v>418</v>
+      </c>
+      <c r="D54" t="s">
         <v>450</v>
-      </c>
-      <c r="C54" t="s">
-        <v>419</v>
-      </c>
-      <c r="D54" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -3649,7 +3649,7 @@
         <v>190</v>
       </c>
       <c r="C55" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D55" t="s">
         <v>191</v>
@@ -3663,7 +3663,7 @@
         <v>192</v>
       </c>
       <c r="C56" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D56" t="s">
         <v>193</v>
@@ -3674,13 +3674,13 @@
         <v>62</v>
       </c>
       <c r="B57" t="s">
+        <v>582</v>
+      </c>
+      <c r="C57" t="s">
+        <v>418</v>
+      </c>
+      <c r="D57" t="s">
         <v>583</v>
-      </c>
-      <c r="C57" t="s">
-        <v>419</v>
-      </c>
-      <c r="D57" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -3688,13 +3688,13 @@
         <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C58" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D58" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -3705,7 +3705,7 @@
         <v>194</v>
       </c>
       <c r="C59" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D59" t="s">
         <v>195</v>
@@ -3719,7 +3719,7 @@
         <v>196</v>
       </c>
       <c r="C60" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D60" t="s">
         <v>197</v>
@@ -3730,13 +3730,13 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C61" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D61" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -3747,7 +3747,7 @@
         <v>198</v>
       </c>
       <c r="C62" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D62" t="s">
         <v>199</v>
@@ -3761,7 +3761,7 @@
         <v>200</v>
       </c>
       <c r="C63" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D63" t="s">
         <v>201</v>
@@ -3775,7 +3775,7 @@
         <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D64" t="s">
         <v>64</v>
@@ -3789,7 +3789,7 @@
         <v>202</v>
       </c>
       <c r="C65" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D65" t="s">
         <v>203</v>
@@ -3803,7 +3803,7 @@
         <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D66" t="s">
         <v>66</v>
@@ -3817,7 +3817,7 @@
         <v>204</v>
       </c>
       <c r="C67" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D67" t="s">
         <v>205</v>
@@ -3831,7 +3831,7 @@
         <v>206</v>
       </c>
       <c r="C68" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D68" t="s">
         <v>207</v>
@@ -3845,7 +3845,7 @@
         <v>208</v>
       </c>
       <c r="C69" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D69" t="s">
         <v>209</v>
@@ -3859,7 +3859,7 @@
         <v>210</v>
       </c>
       <c r="C70" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D70" t="s">
         <v>211</v>
@@ -3873,7 +3873,7 @@
         <v>67</v>
       </c>
       <c r="C71" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D71" t="s">
         <v>68</v>
@@ -3887,7 +3887,7 @@
         <v>212</v>
       </c>
       <c r="C72" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D72" t="s">
         <v>213</v>
@@ -3901,7 +3901,7 @@
         <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D73" t="s">
         <v>70</v>
@@ -3915,7 +3915,7 @@
         <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D74" t="s">
         <v>72</v>
@@ -3929,7 +3929,7 @@
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D75" t="s">
         <v>74</v>
@@ -3943,7 +3943,7 @@
         <v>214</v>
       </c>
       <c r="C76" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D76" t="s">
         <v>215</v>
@@ -3954,13 +3954,13 @@
         <v>62</v>
       </c>
       <c r="B77" t="s">
+        <v>559</v>
+      </c>
+      <c r="C77" t="s">
+        <v>418</v>
+      </c>
+      <c r="D77" t="s">
         <v>560</v>
-      </c>
-      <c r="C77" t="s">
-        <v>419</v>
-      </c>
-      <c r="D77" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -3971,7 +3971,7 @@
         <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D78" t="s">
         <v>76</v>
@@ -3985,7 +3985,7 @@
         <v>216</v>
       </c>
       <c r="C79" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D79" t="s">
         <v>217</v>
@@ -3999,7 +3999,7 @@
         <v>218</v>
       </c>
       <c r="C80" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D80" t="s">
         <v>219</v>
@@ -4010,13 +4010,13 @@
         <v>62</v>
       </c>
       <c r="B81" t="s">
+        <v>470</v>
+      </c>
+      <c r="C81" t="s">
+        <v>418</v>
+      </c>
+      <c r="D81" t="s">
         <v>471</v>
-      </c>
-      <c r="C81" t="s">
-        <v>419</v>
-      </c>
-      <c r="D81" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -4027,7 +4027,7 @@
         <v>220</v>
       </c>
       <c r="C82" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D82" t="s">
         <v>221</v>
@@ -4041,7 +4041,7 @@
         <v>222</v>
       </c>
       <c r="C83" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D83" t="s">
         <v>223</v>
@@ -4055,7 +4055,7 @@
         <v>224</v>
       </c>
       <c r="C84" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D84" t="s">
         <v>225</v>
@@ -4069,7 +4069,7 @@
         <v>77</v>
       </c>
       <c r="C85" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D85" t="s">
         <v>78</v>
@@ -4083,7 +4083,7 @@
         <v>226</v>
       </c>
       <c r="C86" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D86" t="s">
         <v>227</v>
@@ -4097,7 +4097,7 @@
         <v>80</v>
       </c>
       <c r="C87" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D87" t="s">
         <v>81</v>
@@ -4111,7 +4111,7 @@
         <v>228</v>
       </c>
       <c r="C88" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D88" t="s">
         <v>229</v>
@@ -4125,7 +4125,7 @@
         <v>230</v>
       </c>
       <c r="C89" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D89" t="s">
         <v>231</v>
@@ -4139,7 +4139,7 @@
         <v>83</v>
       </c>
       <c r="C90" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D90" t="s">
         <v>84</v>
@@ -4153,7 +4153,7 @@
         <v>232</v>
       </c>
       <c r="C91" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D91" t="s">
         <v>233</v>
@@ -4167,7 +4167,7 @@
         <v>85</v>
       </c>
       <c r="C92" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D92" t="s">
         <v>86</v>
@@ -4178,13 +4178,13 @@
         <v>82</v>
       </c>
       <c r="B93" t="s">
+        <v>576</v>
+      </c>
+      <c r="C93" t="s">
+        <v>418</v>
+      </c>
+      <c r="D93" t="s">
         <v>577</v>
-      </c>
-      <c r="C93" t="s">
-        <v>419</v>
-      </c>
-      <c r="D93" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -4195,7 +4195,7 @@
         <v>234</v>
       </c>
       <c r="C94" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D94" t="s">
         <v>235</v>
@@ -4209,7 +4209,7 @@
         <v>236</v>
       </c>
       <c r="C95" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D95" t="s">
         <v>237</v>
@@ -4223,7 +4223,7 @@
         <v>87</v>
       </c>
       <c r="C96" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D96" t="s">
         <v>88</v>
@@ -4237,7 +4237,7 @@
         <v>89</v>
       </c>
       <c r="C97" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D97" t="s">
         <v>90</v>
@@ -4251,7 +4251,7 @@
         <v>238</v>
       </c>
       <c r="C98" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D98" t="s">
         <v>239</v>
@@ -4265,7 +4265,7 @@
         <v>124</v>
       </c>
       <c r="C99" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D99" t="s">
         <v>125</v>
@@ -4279,7 +4279,7 @@
         <v>240</v>
       </c>
       <c r="C100" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D100" t="s">
         <v>241</v>
@@ -4293,7 +4293,7 @@
         <v>242</v>
       </c>
       <c r="C101" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D101" t="s">
         <v>243</v>
@@ -4307,7 +4307,7 @@
         <v>244</v>
       </c>
       <c r="C102" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D102" t="s">
         <v>245</v>
@@ -4321,7 +4321,7 @@
         <v>91</v>
       </c>
       <c r="C103" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D103" t="s">
         <v>92</v>
@@ -4335,7 +4335,7 @@
         <v>246</v>
       </c>
       <c r="C104" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D104" t="s">
         <v>247</v>
@@ -4349,7 +4349,7 @@
         <v>248</v>
       </c>
       <c r="C105" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D105" t="s">
         <v>249</v>
@@ -4363,7 +4363,7 @@
         <v>250</v>
       </c>
       <c r="C106" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D106" t="s">
         <v>251</v>
@@ -4377,7 +4377,7 @@
         <v>93</v>
       </c>
       <c r="C107" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D107" t="s">
         <v>94</v>
@@ -4391,7 +4391,7 @@
         <v>95</v>
       </c>
       <c r="C108" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D108" t="s">
         <v>96</v>
@@ -4405,7 +4405,7 @@
         <v>252</v>
       </c>
       <c r="C109" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D109" t="s">
         <v>253</v>
@@ -4419,7 +4419,7 @@
         <v>97</v>
       </c>
       <c r="C110" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D110" t="s">
         <v>98</v>
@@ -4433,7 +4433,7 @@
         <v>99</v>
       </c>
       <c r="C111" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D111" t="s">
         <v>100</v>
@@ -4447,7 +4447,7 @@
         <v>101</v>
       </c>
       <c r="C112" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D112" t="s">
         <v>102</v>
@@ -4461,10 +4461,10 @@
         <v>103</v>
       </c>
       <c r="C113" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D113" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -4475,7 +4475,7 @@
         <v>104</v>
       </c>
       <c r="C114" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D114" t="s">
         <v>105</v>
@@ -4489,7 +4489,7 @@
         <v>254</v>
       </c>
       <c r="C115" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D115" t="s">
         <v>255</v>
@@ -4503,7 +4503,7 @@
         <v>256</v>
       </c>
       <c r="C116" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D116" t="s">
         <v>257</v>
@@ -4517,7 +4517,7 @@
         <v>258</v>
       </c>
       <c r="C117" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D117" t="s">
         <v>259</v>
@@ -4531,7 +4531,7 @@
         <v>260</v>
       </c>
       <c r="C118" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D118" t="s">
         <v>261</v>
@@ -4545,7 +4545,7 @@
         <v>106</v>
       </c>
       <c r="C119" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D119" t="s">
         <v>107</v>
@@ -4559,7 +4559,7 @@
         <v>108</v>
       </c>
       <c r="C120" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D120" t="s">
         <v>109</v>
@@ -4573,7 +4573,7 @@
         <v>262</v>
       </c>
       <c r="C121" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D121" t="s">
         <v>263</v>
@@ -4587,7 +4587,7 @@
         <v>264</v>
       </c>
       <c r="C122" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D122" t="s">
         <v>265</v>
@@ -4601,7 +4601,7 @@
         <v>267</v>
       </c>
       <c r="C123" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D123" t="s">
         <v>268</v>
@@ -4615,7 +4615,7 @@
         <v>269</v>
       </c>
       <c r="C124" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D124" t="s">
         <v>270</v>
@@ -4629,7 +4629,7 @@
         <v>271</v>
       </c>
       <c r="C125" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D125" t="s">
         <v>272</v>
@@ -4643,7 +4643,7 @@
         <v>273</v>
       </c>
       <c r="C126" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D126" t="s">
         <v>274</v>
@@ -4657,7 +4657,7 @@
         <v>275</v>
       </c>
       <c r="C127" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D127" t="s">
         <v>276</v>
@@ -4671,7 +4671,7 @@
         <v>10</v>
       </c>
       <c r="C128" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D128" t="s">
         <v>278</v>
@@ -4685,7 +4685,7 @@
         <v>279</v>
       </c>
       <c r="C129" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D129" t="s">
         <v>280</v>
@@ -4699,7 +4699,7 @@
         <v>281</v>
       </c>
       <c r="C130" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D130" t="s">
         <v>282</v>
@@ -4713,7 +4713,7 @@
         <v>283</v>
       </c>
       <c r="C131" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D131" t="s">
         <v>284</v>
@@ -4727,7 +4727,7 @@
         <v>285</v>
       </c>
       <c r="C132" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D132" t="s">
         <v>286</v>
@@ -4741,7 +4741,7 @@
         <v>287</v>
       </c>
       <c r="C133" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D133" t="s">
         <v>288</v>
@@ -4755,7 +4755,7 @@
         <v>289</v>
       </c>
       <c r="C134" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D134" t="s">
         <v>290</v>
@@ -4769,10 +4769,10 @@
         <v>291</v>
       </c>
       <c r="C135" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D135" t="s">
-        <v>292</v>
+        <v>663</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -4780,13 +4780,13 @@
         <v>277</v>
       </c>
       <c r="B136" t="s">
+        <v>292</v>
+      </c>
+      <c r="C136" t="s">
+        <v>418</v>
+      </c>
+      <c r="D136" t="s">
         <v>293</v>
-      </c>
-      <c r="C136" t="s">
-        <v>419</v>
-      </c>
-      <c r="D136" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -4794,13 +4794,13 @@
         <v>277</v>
       </c>
       <c r="B137" t="s">
+        <v>294</v>
+      </c>
+      <c r="C137" t="s">
+        <v>418</v>
+      </c>
+      <c r="D137" t="s">
         <v>295</v>
-      </c>
-      <c r="C137" t="s">
-        <v>419</v>
-      </c>
-      <c r="D137" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -4808,13 +4808,13 @@
         <v>277</v>
       </c>
       <c r="B138" t="s">
+        <v>296</v>
+      </c>
+      <c r="C138" t="s">
+        <v>418</v>
+      </c>
+      <c r="D138" t="s">
         <v>297</v>
-      </c>
-      <c r="C138" t="s">
-        <v>419</v>
-      </c>
-      <c r="D138" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -4822,13 +4822,13 @@
         <v>277</v>
       </c>
       <c r="B139" t="s">
+        <v>298</v>
+      </c>
+      <c r="C139" t="s">
+        <v>418</v>
+      </c>
+      <c r="D139" t="s">
         <v>299</v>
-      </c>
-      <c r="C139" t="s">
-        <v>419</v>
-      </c>
-      <c r="D139" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -4836,13 +4836,13 @@
         <v>277</v>
       </c>
       <c r="B140" t="s">
+        <v>300</v>
+      </c>
+      <c r="C140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D140" t="s">
         <v>301</v>
-      </c>
-      <c r="C140" t="s">
-        <v>419</v>
-      </c>
-      <c r="D140" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -4850,13 +4850,13 @@
         <v>277</v>
       </c>
       <c r="B141" t="s">
+        <v>302</v>
+      </c>
+      <c r="C141" t="s">
+        <v>418</v>
+      </c>
+      <c r="D141" t="s">
         <v>303</v>
-      </c>
-      <c r="C141" t="s">
-        <v>419</v>
-      </c>
-      <c r="D141" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -4864,13 +4864,13 @@
         <v>277</v>
       </c>
       <c r="B142" t="s">
+        <v>304</v>
+      </c>
+      <c r="C142" t="s">
+        <v>418</v>
+      </c>
+      <c r="D142" t="s">
         <v>305</v>
-      </c>
-      <c r="C142" t="s">
-        <v>419</v>
-      </c>
-      <c r="D142" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -4878,13 +4878,13 @@
         <v>277</v>
       </c>
       <c r="B143" t="s">
+        <v>447</v>
+      </c>
+      <c r="C143" t="s">
+        <v>418</v>
+      </c>
+      <c r="D143" t="s">
         <v>448</v>
-      </c>
-      <c r="C143" t="s">
-        <v>419</v>
-      </c>
-      <c r="D143" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -4892,13 +4892,13 @@
         <v>277</v>
       </c>
       <c r="B144" t="s">
+        <v>459</v>
+      </c>
+      <c r="C144" t="s">
+        <v>418</v>
+      </c>
+      <c r="D144" t="s">
         <v>460</v>
-      </c>
-      <c r="C144" t="s">
-        <v>419</v>
-      </c>
-      <c r="D144" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -4906,13 +4906,13 @@
         <v>277</v>
       </c>
       <c r="B145" t="s">
+        <v>306</v>
+      </c>
+      <c r="C145" t="s">
+        <v>418</v>
+      </c>
+      <c r="D145" t="s">
         <v>307</v>
-      </c>
-      <c r="C145" t="s">
-        <v>419</v>
-      </c>
-      <c r="D145" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -4920,13 +4920,13 @@
         <v>277</v>
       </c>
       <c r="B146" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C146" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D146" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -4934,13 +4934,13 @@
         <v>277</v>
       </c>
       <c r="B147" t="s">
+        <v>308</v>
+      </c>
+      <c r="C147" t="s">
+        <v>418</v>
+      </c>
+      <c r="D147" t="s">
         <v>309</v>
-      </c>
-      <c r="C147" t="s">
-        <v>419</v>
-      </c>
-      <c r="D147" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -4948,13 +4948,13 @@
         <v>277</v>
       </c>
       <c r="B148" t="s">
+        <v>310</v>
+      </c>
+      <c r="C148" t="s">
+        <v>418</v>
+      </c>
+      <c r="D148" t="s">
         <v>311</v>
-      </c>
-      <c r="C148" t="s">
-        <v>419</v>
-      </c>
-      <c r="D148" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -4962,13 +4962,13 @@
         <v>277</v>
       </c>
       <c r="B149" t="s">
+        <v>312</v>
+      </c>
+      <c r="C149" t="s">
+        <v>418</v>
+      </c>
+      <c r="D149" t="s">
         <v>313</v>
-      </c>
-      <c r="C149" t="s">
-        <v>419</v>
-      </c>
-      <c r="D149" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -4976,13 +4976,13 @@
         <v>277</v>
       </c>
       <c r="B150" t="s">
+        <v>314</v>
+      </c>
+      <c r="C150" t="s">
+        <v>418</v>
+      </c>
+      <c r="D150" t="s">
         <v>315</v>
-      </c>
-      <c r="C150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D150" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -4990,13 +4990,13 @@
         <v>277</v>
       </c>
       <c r="B151" t="s">
+        <v>316</v>
+      </c>
+      <c r="C151" t="s">
+        <v>418</v>
+      </c>
+      <c r="D151" t="s">
         <v>317</v>
-      </c>
-      <c r="C151" t="s">
-        <v>419</v>
-      </c>
-      <c r="D151" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -5004,13 +5004,13 @@
         <v>277</v>
       </c>
       <c r="B152" t="s">
+        <v>318</v>
+      </c>
+      <c r="C152" t="s">
+        <v>418</v>
+      </c>
+      <c r="D152" t="s">
         <v>319</v>
-      </c>
-      <c r="C152" t="s">
-        <v>419</v>
-      </c>
-      <c r="D152" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -5018,13 +5018,13 @@
         <v>277</v>
       </c>
       <c r="B153" t="s">
+        <v>462</v>
+      </c>
+      <c r="C153" t="s">
+        <v>418</v>
+      </c>
+      <c r="D153" t="s">
         <v>463</v>
-      </c>
-      <c r="C153" t="s">
-        <v>419</v>
-      </c>
-      <c r="D153" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -5032,13 +5032,13 @@
         <v>277</v>
       </c>
       <c r="B154" t="s">
+        <v>320</v>
+      </c>
+      <c r="C154" t="s">
+        <v>418</v>
+      </c>
+      <c r="D154" t="s">
         <v>321</v>
-      </c>
-      <c r="C154" t="s">
-        <v>419</v>
-      </c>
-      <c r="D154" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -5046,13 +5046,13 @@
         <v>277</v>
       </c>
       <c r="B155" t="s">
+        <v>322</v>
+      </c>
+      <c r="C155" t="s">
+        <v>418</v>
+      </c>
+      <c r="D155" t="s">
         <v>323</v>
-      </c>
-      <c r="C155" t="s">
-        <v>419</v>
-      </c>
-      <c r="D155" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -5060,13 +5060,13 @@
         <v>277</v>
       </c>
       <c r="B156" t="s">
+        <v>324</v>
+      </c>
+      <c r="C156" t="s">
+        <v>418</v>
+      </c>
+      <c r="D156" t="s">
         <v>325</v>
-      </c>
-      <c r="C156" t="s">
-        <v>419</v>
-      </c>
-      <c r="D156" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -5074,13 +5074,13 @@
         <v>277</v>
       </c>
       <c r="B157" t="s">
+        <v>326</v>
+      </c>
+      <c r="C157" t="s">
+        <v>418</v>
+      </c>
+      <c r="D157" t="s">
         <v>327</v>
-      </c>
-      <c r="C157" t="s">
-        <v>419</v>
-      </c>
-      <c r="D157" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -5088,13 +5088,13 @@
         <v>277</v>
       </c>
       <c r="B158" t="s">
+        <v>328</v>
+      </c>
+      <c r="C158" t="s">
+        <v>418</v>
+      </c>
+      <c r="D158" t="s">
         <v>329</v>
-      </c>
-      <c r="C158" t="s">
-        <v>419</v>
-      </c>
-      <c r="D158" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -5102,13 +5102,13 @@
         <v>277</v>
       </c>
       <c r="B159" t="s">
+        <v>330</v>
+      </c>
+      <c r="C159" t="s">
+        <v>418</v>
+      </c>
+      <c r="D159" t="s">
         <v>331</v>
-      </c>
-      <c r="C159" t="s">
-        <v>419</v>
-      </c>
-      <c r="D159" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -5116,13 +5116,13 @@
         <v>277</v>
       </c>
       <c r="B160" t="s">
+        <v>442</v>
+      </c>
+      <c r="C160" t="s">
+        <v>418</v>
+      </c>
+      <c r="D160" t="s">
         <v>443</v>
-      </c>
-      <c r="C160" t="s">
-        <v>419</v>
-      </c>
-      <c r="D160" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -5130,125 +5130,125 @@
         <v>277</v>
       </c>
       <c r="B161" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C161" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D161" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>597</v>
+      </c>
+      <c r="B162" t="s">
         <v>598</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" t="s">
+        <v>418</v>
+      </c>
+      <c r="D162" t="s">
         <v>599</v>
-      </c>
-      <c r="C162" t="s">
-        <v>419</v>
-      </c>
-      <c r="D162" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>611</v>
+      </c>
+      <c r="B163" t="s">
         <v>612</v>
       </c>
-      <c r="B163" t="s">
-        <v>613</v>
-      </c>
       <c r="C163" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D163" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B164" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C164" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D164" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>609</v>
+      </c>
+      <c r="B165" t="s">
         <v>610</v>
       </c>
-      <c r="B165" t="s">
-        <v>611</v>
-      </c>
       <c r="C165" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D165" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B166" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C166" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D166" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B167" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C167" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D167" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>332</v>
+      </c>
+      <c r="B168" t="s">
         <v>333</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
+        <v>418</v>
+      </c>
+      <c r="D168" t="s">
         <v>334</v>
-      </c>
-      <c r="C168" t="s">
-        <v>419</v>
-      </c>
-      <c r="D168" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B169" t="s">
+        <v>335</v>
+      </c>
+      <c r="C169" t="s">
+        <v>418</v>
+      </c>
+      <c r="D169" t="s">
         <v>336</v>
-      </c>
-      <c r="C169" t="s">
-        <v>419</v>
-      </c>
-      <c r="D169" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -5259,7 +5259,7 @@
         <v>111</v>
       </c>
       <c r="C170" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D170" t="s">
         <v>112</v>
@@ -5270,13 +5270,13 @@
         <v>110</v>
       </c>
       <c r="B171" t="s">
+        <v>337</v>
+      </c>
+      <c r="C171" t="s">
+        <v>418</v>
+      </c>
+      <c r="D171" t="s">
         <v>338</v>
-      </c>
-      <c r="C171" t="s">
-        <v>419</v>
-      </c>
-      <c r="D171" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -5287,7 +5287,7 @@
         <v>114</v>
       </c>
       <c r="C172" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D172" t="s">
         <v>115</v>
@@ -5298,13 +5298,13 @@
         <v>113</v>
       </c>
       <c r="B173" t="s">
+        <v>339</v>
+      </c>
+      <c r="C173" t="s">
+        <v>418</v>
+      </c>
+      <c r="D173" t="s">
         <v>340</v>
-      </c>
-      <c r="C173" t="s">
-        <v>419</v>
-      </c>
-      <c r="D173" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -5315,7 +5315,7 @@
         <v>116</v>
       </c>
       <c r="C174" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D174" t="s">
         <v>117</v>
@@ -5326,13 +5326,13 @@
         <v>113</v>
       </c>
       <c r="B175" t="s">
+        <v>341</v>
+      </c>
+      <c r="C175" t="s">
+        <v>418</v>
+      </c>
+      <c r="D175" t="s">
         <v>342</v>
-      </c>
-      <c r="C175" t="s">
-        <v>419</v>
-      </c>
-      <c r="D175" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -5343,7 +5343,7 @@
         <v>118</v>
       </c>
       <c r="C176" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D176" t="s">
         <v>119</v>
@@ -5354,13 +5354,13 @@
         <v>113</v>
       </c>
       <c r="B177" t="s">
+        <v>343</v>
+      </c>
+      <c r="C177" t="s">
+        <v>418</v>
+      </c>
+      <c r="D177" t="s">
         <v>344</v>
-      </c>
-      <c r="C177" t="s">
-        <v>419</v>
-      </c>
-      <c r="D177" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -5368,13 +5368,13 @@
         <v>113</v>
       </c>
       <c r="B178" t="s">
+        <v>345</v>
+      </c>
+      <c r="C178" t="s">
+        <v>418</v>
+      </c>
+      <c r="D178" t="s">
         <v>346</v>
-      </c>
-      <c r="C178" t="s">
-        <v>419</v>
-      </c>
-      <c r="D178" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -5382,13 +5382,13 @@
         <v>113</v>
       </c>
       <c r="B179" t="s">
+        <v>349</v>
+      </c>
+      <c r="C179" t="s">
+        <v>418</v>
+      </c>
+      <c r="D179" t="s">
         <v>350</v>
-      </c>
-      <c r="C179" t="s">
-        <v>419</v>
-      </c>
-      <c r="D179" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -5396,13 +5396,13 @@
         <v>113</v>
       </c>
       <c r="B180" t="s">
+        <v>347</v>
+      </c>
+      <c r="C180" t="s">
+        <v>418</v>
+      </c>
+      <c r="D180" t="s">
         <v>348</v>
-      </c>
-      <c r="C180" t="s">
-        <v>419</v>
-      </c>
-      <c r="D180" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -5413,7 +5413,7 @@
         <v>121</v>
       </c>
       <c r="C181" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D181" t="s">
         <v>122</v>
@@ -5424,41 +5424,41 @@
         <v>120</v>
       </c>
       <c r="B182" t="s">
+        <v>351</v>
+      </c>
+      <c r="C182" t="s">
+        <v>418</v>
+      </c>
+      <c r="D182" t="s">
         <v>352</v>
-      </c>
-      <c r="C182" t="s">
-        <v>419</v>
-      </c>
-      <c r="D182" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
+        <v>514</v>
+      </c>
+      <c r="B183" t="s">
         <v>515</v>
       </c>
-      <c r="B183" t="s">
+      <c r="C183" t="s">
+        <v>418</v>
+      </c>
+      <c r="D183" t="s">
         <v>516</v>
-      </c>
-      <c r="C183" t="s">
-        <v>419</v>
-      </c>
-      <c r="D183" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
+        <v>604</v>
+      </c>
+      <c r="B184" t="s">
         <v>605</v>
       </c>
-      <c r="B184" t="s">
-        <v>606</v>
-      </c>
       <c r="C184" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D184" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -5466,13 +5466,13 @@
         <v>126</v>
       </c>
       <c r="B185" t="s">
+        <v>353</v>
+      </c>
+      <c r="C185" t="s">
+        <v>418</v>
+      </c>
+      <c r="D185" t="s">
         <v>354</v>
-      </c>
-      <c r="C185" t="s">
-        <v>419</v>
-      </c>
-      <c r="D185" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -5483,7 +5483,7 @@
         <v>127</v>
       </c>
       <c r="C186" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D186" t="s">
         <v>128</v>
@@ -5494,13 +5494,13 @@
         <v>126</v>
       </c>
       <c r="B187" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C187" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D187" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -5508,13 +5508,13 @@
         <v>126</v>
       </c>
       <c r="B188" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C188" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D188" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -5522,13 +5522,13 @@
         <v>126</v>
       </c>
       <c r="B189" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C189" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D189" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -5536,13 +5536,13 @@
         <v>126</v>
       </c>
       <c r="B190" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C190" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D190" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -5550,13 +5550,13 @@
         <v>126</v>
       </c>
       <c r="B191" t="s">
+        <v>355</v>
+      </c>
+      <c r="C191" t="s">
+        <v>418</v>
+      </c>
+      <c r="D191" t="s">
         <v>356</v>
-      </c>
-      <c r="C191" t="s">
-        <v>419</v>
-      </c>
-      <c r="D191" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
@@ -5567,7 +5567,7 @@
         <v>129</v>
       </c>
       <c r="C192" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D192" t="s">
         <v>130</v>
@@ -5575,16 +5575,16 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>357</v>
+      </c>
+      <c r="B193" t="s">
         <v>358</v>
       </c>
-      <c r="B193" t="s">
+      <c r="C193" t="s">
+        <v>418</v>
+      </c>
+      <c r="D193" t="s">
         <v>359</v>
-      </c>
-      <c r="C193" t="s">
-        <v>419</v>
-      </c>
-      <c r="D193" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -5595,7 +5595,7 @@
         <v>132</v>
       </c>
       <c r="C194" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D194" t="s">
         <v>133</v>
@@ -5606,13 +5606,13 @@
         <v>131</v>
       </c>
       <c r="B195" t="s">
+        <v>360</v>
+      </c>
+      <c r="C195" t="s">
+        <v>418</v>
+      </c>
+      <c r="D195" t="s">
         <v>361</v>
-      </c>
-      <c r="C195" t="s">
-        <v>419</v>
-      </c>
-      <c r="D195" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -5623,7 +5623,7 @@
         <v>134</v>
       </c>
       <c r="C196" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D196" t="s">
         <v>135</v>
@@ -5637,7 +5637,7 @@
         <v>136</v>
       </c>
       <c r="C197" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D197" t="s">
         <v>137</v>
@@ -5648,13 +5648,13 @@
         <v>131</v>
       </c>
       <c r="B198" t="s">
+        <v>362</v>
+      </c>
+      <c r="C198" t="s">
+        <v>418</v>
+      </c>
+      <c r="D198" t="s">
         <v>363</v>
-      </c>
-      <c r="C198" t="s">
-        <v>419</v>
-      </c>
-      <c r="D198" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -5665,38 +5665,38 @@
         <v>138</v>
       </c>
       <c r="C199" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D199" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>364</v>
+      </c>
+      <c r="B200" t="s">
         <v>365</v>
       </c>
-      <c r="B200" t="s">
+      <c r="C200" t="s">
+        <v>418</v>
+      </c>
+      <c r="D200" t="s">
         <v>366</v>
-      </c>
-      <c r="C200" t="s">
-        <v>419</v>
-      </c>
-      <c r="D200" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B201" t="s">
+        <v>367</v>
+      </c>
+      <c r="C201" t="s">
+        <v>418</v>
+      </c>
+      <c r="D201" t="s">
         <v>368</v>
-      </c>
-      <c r="C201" t="s">
-        <v>419</v>
-      </c>
-      <c r="D201" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -5707,7 +5707,7 @@
         <v>142</v>
       </c>
       <c r="C202" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D202" t="s">
         <v>143</v>
@@ -5721,7 +5721,7 @@
         <v>140</v>
       </c>
       <c r="C203" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D203" t="s">
         <v>141</v>
@@ -5729,688 +5729,688 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>521</v>
+      </c>
+      <c r="B204" t="s">
         <v>522</v>
       </c>
-      <c r="B204" t="s">
+      <c r="C204" t="s">
+        <v>418</v>
+      </c>
+      <c r="D204" t="s">
         <v>523</v>
-      </c>
-      <c r="C204" t="s">
-        <v>419</v>
-      </c>
-      <c r="D204" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B205" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C205" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D205" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
+        <v>421</v>
+      </c>
+      <c r="B206" t="s">
         <v>422</v>
       </c>
-      <c r="B206" t="s">
-        <v>423</v>
-      </c>
       <c r="C206" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D206" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B207" t="s">
+        <v>506</v>
+      </c>
+      <c r="C207" t="s">
+        <v>418</v>
+      </c>
+      <c r="D207" t="s">
         <v>507</v>
-      </c>
-      <c r="C207" t="s">
-        <v>419</v>
-      </c>
-      <c r="D207" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B208" t="s">
+        <v>524</v>
+      </c>
+      <c r="C208" t="s">
+        <v>418</v>
+      </c>
+      <c r="D208" t="s">
         <v>525</v>
-      </c>
-      <c r="C208" t="s">
-        <v>419</v>
-      </c>
-      <c r="D208" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B209" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C209" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D209" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B210" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C210" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D210" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B211" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C211" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D211" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B212" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C212" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D212" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B213" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C213" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D213" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B214" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C214" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D214" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B215" t="s">
+        <v>453</v>
+      </c>
+      <c r="C215" t="s">
+        <v>418</v>
+      </c>
+      <c r="D215" t="s">
         <v>454</v>
-      </c>
-      <c r="C215" t="s">
-        <v>419</v>
-      </c>
-      <c r="D215" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B216" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C216" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D216" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B217" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C217" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D217" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B218" t="s">
+        <v>510</v>
+      </c>
+      <c r="C218" t="s">
+        <v>418</v>
+      </c>
+      <c r="D218" t="s">
         <v>511</v>
-      </c>
-      <c r="C218" t="s">
-        <v>419</v>
-      </c>
-      <c r="D218" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B219" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C219" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D219" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B220" t="s">
+        <v>512</v>
+      </c>
+      <c r="C220" t="s">
+        <v>418</v>
+      </c>
+      <c r="D220" t="s">
         <v>513</v>
-      </c>
-      <c r="C220" t="s">
-        <v>419</v>
-      </c>
-      <c r="D220" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B221" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C221" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D221" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B222" t="s">
+        <v>468</v>
+      </c>
+      <c r="C222" t="s">
+        <v>418</v>
+      </c>
+      <c r="D222" t="s">
         <v>469</v>
-      </c>
-      <c r="C222" t="s">
-        <v>419</v>
-      </c>
-      <c r="D222" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B223" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C223" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D223" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B224" t="s">
+        <v>465</v>
+      </c>
+      <c r="C224" t="s">
+        <v>418</v>
+      </c>
+      <c r="D224" t="s">
         <v>466</v>
-      </c>
-      <c r="C224" t="s">
-        <v>419</v>
-      </c>
-      <c r="D224" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B225" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C225" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D225" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B226" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C226" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D226" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B227" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C227" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D227" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B228" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C228" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D228" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B229" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C229" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D229" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B230" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C230" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D230" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B231" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C231" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D231" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B232" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C232" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D232" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B233" t="s">
+        <v>519</v>
+      </c>
+      <c r="C233" t="s">
+        <v>418</v>
+      </c>
+      <c r="D233" t="s">
         <v>520</v>
-      </c>
-      <c r="C233" t="s">
-        <v>419</v>
-      </c>
-      <c r="D233" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B234" t="s">
+        <v>451</v>
+      </c>
+      <c r="C234" t="s">
+        <v>418</v>
+      </c>
+      <c r="D234" t="s">
         <v>452</v>
-      </c>
-      <c r="C234" t="s">
-        <v>419</v>
-      </c>
-      <c r="D234" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B235" t="s">
+        <v>517</v>
+      </c>
+      <c r="C235" t="s">
+        <v>418</v>
+      </c>
+      <c r="D235" t="s">
         <v>518</v>
-      </c>
-      <c r="C235" t="s">
-        <v>419</v>
-      </c>
-      <c r="D235" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B236" t="s">
+        <v>455</v>
+      </c>
+      <c r="C236" t="s">
+        <v>418</v>
+      </c>
+      <c r="D236" t="s">
         <v>456</v>
-      </c>
-      <c r="C236" t="s">
-        <v>419</v>
-      </c>
-      <c r="D236" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
+        <v>602</v>
+      </c>
+      <c r="B237" t="s">
         <v>603</v>
       </c>
-      <c r="B237" t="s">
-        <v>604</v>
-      </c>
       <c r="C237" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D237" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B238" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C238" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D238" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
+        <v>615</v>
+      </c>
+      <c r="B239" t="s">
         <v>616</v>
       </c>
-      <c r="B239" t="s">
-        <v>617</v>
-      </c>
       <c r="C239" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D239" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B240" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C240" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D240" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
+        <v>620</v>
+      </c>
+      <c r="B241" t="s">
         <v>621</v>
       </c>
-      <c r="B241" t="s">
-        <v>622</v>
-      </c>
       <c r="C241" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D241" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B242" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C242" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D242" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
+        <v>628</v>
+      </c>
+      <c r="B243" t="s">
         <v>629</v>
       </c>
-      <c r="B243" t="s">
-        <v>630</v>
-      </c>
       <c r="C243" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D243" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B244" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C244" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D244" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B245" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C245" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D245" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
+        <v>369</v>
+      </c>
+      <c r="B246" t="s">
         <v>370</v>
       </c>
-      <c r="B246" t="s">
+      <c r="C246" t="s">
+        <v>418</v>
+      </c>
+      <c r="D246" t="s">
         <v>371</v>
-      </c>
-      <c r="C246" t="s">
-        <v>419</v>
-      </c>
-      <c r="D246" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B247" t="s">
+        <v>584</v>
+      </c>
+      <c r="C247" t="s">
+        <v>418</v>
+      </c>
+      <c r="D247" t="s">
         <v>585</v>
-      </c>
-      <c r="C247" t="s">
-        <v>419</v>
-      </c>
-      <c r="D247" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B248" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C248" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D248" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B249" t="s">
+        <v>372</v>
+      </c>
+      <c r="C249" t="s">
+        <v>418</v>
+      </c>
+      <c r="D249" t="s">
         <v>373</v>
-      </c>
-      <c r="C249" t="s">
-        <v>419</v>
-      </c>
-      <c r="D249" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B250" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C250" t="s">
+        <v>418</v>
+      </c>
+      <c r="D250" t="s">
         <v>419</v>
-      </c>
-      <c r="D250" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B251" t="s">
+        <v>588</v>
+      </c>
+      <c r="C251" t="s">
+        <v>418</v>
+      </c>
+      <c r="D251" t="s">
         <v>589</v>
-      </c>
-      <c r="C251" t="s">
-        <v>419</v>
-      </c>
-      <c r="D251" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B252" t="s">
+        <v>375</v>
+      </c>
+      <c r="C252" t="s">
+        <v>418</v>
+      </c>
+      <c r="D252" t="s">
         <v>376</v>
-      </c>
-      <c r="C252" t="s">
-        <v>419</v>
-      </c>
-      <c r="D252" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
@@ -6421,7 +6421,7 @@
         <v>145</v>
       </c>
       <c r="C253" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D253" t="s">
         <v>146</v>
@@ -6432,13 +6432,13 @@
         <v>144</v>
       </c>
       <c r="B254" t="s">
+        <v>377</v>
+      </c>
+      <c r="C254" t="s">
+        <v>418</v>
+      </c>
+      <c r="D254" t="s">
         <v>378</v>
-      </c>
-      <c r="C254" t="s">
-        <v>419</v>
-      </c>
-      <c r="D254" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
@@ -6446,13 +6446,13 @@
         <v>144</v>
       </c>
       <c r="B255" t="s">
+        <v>590</v>
+      </c>
+      <c r="C255" t="s">
+        <v>418</v>
+      </c>
+      <c r="D255" t="s">
         <v>591</v>
-      </c>
-      <c r="C255" t="s">
-        <v>419</v>
-      </c>
-      <c r="D255" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
@@ -6460,13 +6460,13 @@
         <v>144</v>
       </c>
       <c r="B256" t="s">
+        <v>379</v>
+      </c>
+      <c r="C256" t="s">
+        <v>418</v>
+      </c>
+      <c r="D256" t="s">
         <v>380</v>
-      </c>
-      <c r="C256" t="s">
-        <v>419</v>
-      </c>
-      <c r="D256" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
@@ -6474,13 +6474,13 @@
         <v>144</v>
       </c>
       <c r="B257" t="s">
+        <v>381</v>
+      </c>
+      <c r="C257" t="s">
+        <v>418</v>
+      </c>
+      <c r="D257" t="s">
         <v>382</v>
-      </c>
-      <c r="C257" t="s">
-        <v>419</v>
-      </c>
-      <c r="D257" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
@@ -6488,13 +6488,13 @@
         <v>144</v>
       </c>
       <c r="B258" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C258" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D258" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
@@ -6502,251 +6502,251 @@
         <v>144</v>
       </c>
       <c r="B259" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C259" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D259" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B260" t="s">
+        <v>600</v>
+      </c>
+      <c r="C260" t="s">
+        <v>418</v>
+      </c>
+      <c r="D260" t="s">
         <v>601</v>
-      </c>
-      <c r="C260" t="s">
-        <v>419</v>
-      </c>
-      <c r="D260" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B261" t="s">
+        <v>578</v>
+      </c>
+      <c r="C261" t="s">
+        <v>418</v>
+      </c>
+      <c r="D261" t="s">
         <v>579</v>
-      </c>
-      <c r="C261" t="s">
-        <v>419</v>
-      </c>
-      <c r="D261" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B262" t="s">
+        <v>580</v>
+      </c>
+      <c r="C262" t="s">
+        <v>418</v>
+      </c>
+      <c r="D262" t="s">
         <v>581</v>
-      </c>
-      <c r="C262" t="s">
-        <v>419</v>
-      </c>
-      <c r="D262" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
+        <v>530</v>
+      </c>
+      <c r="B263" t="s">
         <v>531</v>
       </c>
-      <c r="B263" t="s">
-        <v>532</v>
-      </c>
       <c r="C263" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D263" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B264" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C264" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D264" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B265" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C265" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D265" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B266" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C266" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D266" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B267" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C267" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D267" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B268" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C268" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D268" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B269" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C269" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D269" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B270" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C270" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D270" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B271" t="s">
+        <v>586</v>
+      </c>
+      <c r="C271" t="s">
+        <v>418</v>
+      </c>
+      <c r="D271" t="s">
         <v>587</v>
-      </c>
-      <c r="C271" t="s">
-        <v>419</v>
-      </c>
-      <c r="D271" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B272" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C272" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D272" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B273" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C273" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D273" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B274" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C274" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D274" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B275" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C275" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D275" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B276" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C276" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D276" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
@@ -6754,13 +6754,13 @@
         <v>147</v>
       </c>
       <c r="B277" t="s">
+        <v>457</v>
+      </c>
+      <c r="C277" t="s">
+        <v>418</v>
+      </c>
+      <c r="D277" t="s">
         <v>458</v>
-      </c>
-      <c r="C277" t="s">
-        <v>419</v>
-      </c>
-      <c r="D277" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
@@ -6768,13 +6768,13 @@
         <v>147</v>
       </c>
       <c r="B278" t="s">
+        <v>383</v>
+      </c>
+      <c r="C278" t="s">
+        <v>418</v>
+      </c>
+      <c r="D278" t="s">
         <v>384</v>
-      </c>
-      <c r="C278" t="s">
-        <v>419</v>
-      </c>
-      <c r="D278" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
@@ -6785,7 +6785,7 @@
         <v>147</v>
       </c>
       <c r="C279" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D279" t="s">
         <v>148</v>
@@ -6796,13 +6796,13 @@
         <v>147</v>
       </c>
       <c r="B280" t="s">
+        <v>385</v>
+      </c>
+      <c r="C280" t="s">
+        <v>418</v>
+      </c>
+      <c r="D280" t="s">
         <v>386</v>
-      </c>
-      <c r="C280" t="s">
-        <v>419</v>
-      </c>
-      <c r="D280" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
@@ -6810,13 +6810,13 @@
         <v>149</v>
       </c>
       <c r="B281" t="s">
+        <v>387</v>
+      </c>
+      <c r="C281" t="s">
+        <v>418</v>
+      </c>
+      <c r="D281" t="s">
         <v>388</v>
-      </c>
-      <c r="C281" t="s">
-        <v>419</v>
-      </c>
-      <c r="D281" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
@@ -6824,13 +6824,13 @@
         <v>149</v>
       </c>
       <c r="B282" t="s">
+        <v>389</v>
+      </c>
+      <c r="C282" t="s">
+        <v>418</v>
+      </c>
+      <c r="D282" t="s">
         <v>390</v>
-      </c>
-      <c r="C282" t="s">
-        <v>419</v>
-      </c>
-      <c r="D282" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
@@ -6838,13 +6838,13 @@
         <v>149</v>
       </c>
       <c r="B283" t="s">
+        <v>391</v>
+      </c>
+      <c r="C283" t="s">
+        <v>418</v>
+      </c>
+      <c r="D283" t="s">
         <v>392</v>
-      </c>
-      <c r="C283" t="s">
-        <v>419</v>
-      </c>
-      <c r="D283" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
@@ -6852,13 +6852,13 @@
         <v>149</v>
       </c>
       <c r="B284" t="s">
+        <v>393</v>
+      </c>
+      <c r="C284" t="s">
+        <v>418</v>
+      </c>
+      <c r="D284" t="s">
         <v>394</v>
-      </c>
-      <c r="C284" t="s">
-        <v>419</v>
-      </c>
-      <c r="D284" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
@@ -6866,13 +6866,13 @@
         <v>149</v>
       </c>
       <c r="B285" t="s">
+        <v>395</v>
+      </c>
+      <c r="C285" t="s">
+        <v>418</v>
+      </c>
+      <c r="D285" t="s">
         <v>396</v>
-      </c>
-      <c r="C285" t="s">
-        <v>419</v>
-      </c>
-      <c r="D285" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
@@ -6880,293 +6880,293 @@
         <v>149</v>
       </c>
       <c r="B286" t="s">
+        <v>397</v>
+      </c>
+      <c r="C286" t="s">
+        <v>418</v>
+      </c>
+      <c r="D286" t="s">
         <v>398</v>
-      </c>
-      <c r="C286" t="s">
-        <v>419</v>
-      </c>
-      <c r="D286" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B287" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C287" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D287" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B288" t="s">
+        <v>526</v>
+      </c>
+      <c r="C288" t="s">
+        <v>418</v>
+      </c>
+      <c r="D288" t="s">
         <v>527</v>
-      </c>
-      <c r="C288" t="s">
-        <v>419</v>
-      </c>
-      <c r="D288" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B289" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C289" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D289" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B290" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C290" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D290" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B291" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C291" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D291" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B292" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C292" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D292" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B293" t="s">
+        <v>504</v>
+      </c>
+      <c r="C293" t="s">
+        <v>418</v>
+      </c>
+      <c r="D293" t="s">
         <v>505</v>
-      </c>
-      <c r="C293" t="s">
-        <v>419</v>
-      </c>
-      <c r="D293" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B294" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C294" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D294" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B295" t="s">
+        <v>508</v>
+      </c>
+      <c r="C295" t="s">
+        <v>418</v>
+      </c>
+      <c r="D295" t="s">
         <v>509</v>
-      </c>
-      <c r="C295" t="s">
-        <v>419</v>
-      </c>
-      <c r="D295" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B296" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C296" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D296" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
+        <v>473</v>
+      </c>
+      <c r="B297" t="s">
         <v>474</v>
       </c>
-      <c r="B297" t="s">
-        <v>475</v>
-      </c>
       <c r="C297" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D297" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B298" t="s">
+        <v>528</v>
+      </c>
+      <c r="C298" t="s">
+        <v>418</v>
+      </c>
+      <c r="D298" t="s">
         <v>529</v>
-      </c>
-      <c r="C298" t="s">
-        <v>419</v>
-      </c>
-      <c r="D298" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
+        <v>478</v>
+      </c>
+      <c r="B299" t="s">
         <v>479</v>
       </c>
-      <c r="B299" t="s">
-        <v>480</v>
-      </c>
       <c r="C299" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D299" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
+        <v>399</v>
+      </c>
+      <c r="B300" t="s">
         <v>400</v>
       </c>
-      <c r="B300" t="s">
-        <v>401</v>
-      </c>
       <c r="C300" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D300" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B301" t="s">
+        <v>401</v>
+      </c>
+      <c r="C301" t="s">
+        <v>418</v>
+      </c>
+      <c r="D301" t="s">
         <v>402</v>
-      </c>
-      <c r="C301" t="s">
-        <v>419</v>
-      </c>
-      <c r="D301" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B302" t="s">
+        <v>403</v>
+      </c>
+      <c r="C302" t="s">
+        <v>418</v>
+      </c>
+      <c r="D302" t="s">
         <v>404</v>
-      </c>
-      <c r="C302" t="s">
-        <v>419</v>
-      </c>
-      <c r="D302" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
+        <v>405</v>
+      </c>
+      <c r="B303" t="s">
         <v>406</v>
       </c>
-      <c r="B303" t="s">
+      <c r="C303" t="s">
+        <v>418</v>
+      </c>
+      <c r="D303" t="s">
         <v>407</v>
-      </c>
-      <c r="C303" t="s">
-        <v>419</v>
-      </c>
-      <c r="D303" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B304" t="s">
+        <v>408</v>
+      </c>
+      <c r="C304" t="s">
+        <v>418</v>
+      </c>
+      <c r="D304" t="s">
         <v>409</v>
-      </c>
-      <c r="C304" t="s">
-        <v>419</v>
-      </c>
-      <c r="D304" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B305" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C305" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D305" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
+        <v>554</v>
+      </c>
+      <c r="B306" t="s">
         <v>555</v>
       </c>
-      <c r="B306" t="s">
-        <v>556</v>
-      </c>
       <c r="C306" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D306" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
@@ -7174,13 +7174,13 @@
         <v>150</v>
       </c>
       <c r="B307" t="s">
+        <v>410</v>
+      </c>
+      <c r="C307" t="s">
+        <v>417</v>
+      </c>
+      <c r="D307" t="s">
         <v>411</v>
-      </c>
-      <c r="C307" t="s">
-        <v>418</v>
-      </c>
-      <c r="D307" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
@@ -7188,13 +7188,13 @@
         <v>62</v>
       </c>
       <c r="B308" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C308" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D308" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
@@ -7205,10 +7205,10 @@
         <v>151</v>
       </c>
       <c r="C309" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D309" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
@@ -7216,13 +7216,13 @@
         <v>150</v>
       </c>
       <c r="B310" t="s">
+        <v>412</v>
+      </c>
+      <c r="C310" t="s">
+        <v>418</v>
+      </c>
+      <c r="D310" t="s">
         <v>413</v>
-      </c>
-      <c r="C310" t="s">
-        <v>419</v>
-      </c>
-      <c r="D310" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
@@ -7230,13 +7230,13 @@
         <v>150</v>
       </c>
       <c r="B311" t="s">
+        <v>557</v>
+      </c>
+      <c r="C311" t="s">
+        <v>418</v>
+      </c>
+      <c r="D311" t="s">
         <v>558</v>
-      </c>
-      <c r="C311" t="s">
-        <v>419</v>
-      </c>
-      <c r="D311" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
@@ -7247,7 +7247,7 @@
         <v>152</v>
       </c>
       <c r="C312" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D312" t="s">
         <v>153</v>
@@ -7258,13 +7258,13 @@
         <v>150</v>
       </c>
       <c r="B313" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C313" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D313" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functions through mod 7
</commit_message>
<xml_diff>
--- a/big_functions_frame.xlsx
+++ b/big_functions_frame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ssd980/datasci_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED56A00-F477-3B4D-82A6-BC243C266571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13010EA6-D917-AF41-A07B-317F63082857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21600" yWindow="0" windowWidth="68800" windowHeight="28800" xr2:uid="{95C4795D-FAAA-484B-ACF2-0B904DFB98DD}"/>
+    <workbookView xWindow="21600" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{95C4795D-FAAA-484B-ACF2-0B904DFB98DD}"/>
   </bookViews>
   <sheets>
     <sheet name="big_functions_frame" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="706">
   <si>
     <t>package</t>
   </si>
@@ -2012,6 +2012,132 @@
   </si>
   <si>
     <t>Set upper and lower values of a plot axis based on the range of data</t>
+  </si>
+  <si>
+    <t>nest</t>
+  </si>
+  <si>
+    <t>Collapse variables into a list column</t>
+  </si>
+  <si>
+    <t>unnest</t>
+  </si>
+  <si>
+    <t>Convert a list column to a series of columns, often resulting in additional rows</t>
+  </si>
+  <si>
+    <t>stringi</t>
+  </si>
+  <si>
+    <t>stri_rand_strings</t>
+  </si>
+  <si>
+    <t>Generate a random string of letter and number symbols</t>
+  </si>
+  <si>
+    <t>expand_grid</t>
+  </si>
+  <si>
+    <t>Generate a tibble that includes all potential combinates of two or more vectors</t>
+  </si>
+  <si>
+    <t>DBI</t>
+  </si>
+  <si>
+    <t>dbConnect</t>
+  </si>
+  <si>
+    <t>Establish a connection to a database</t>
+  </si>
+  <si>
+    <t>RSQLite</t>
+  </si>
+  <si>
+    <t>SQLite</t>
+  </si>
+  <si>
+    <t>Connect to an SQLite database</t>
+  </si>
+  <si>
+    <t>dbWriteTable</t>
+  </si>
+  <si>
+    <t>Add a table to a database</t>
+  </si>
+  <si>
+    <t>dbListTables</t>
+  </si>
+  <si>
+    <t>List the tables in a database</t>
+  </si>
+  <si>
+    <t>dblyr</t>
+  </si>
+  <si>
+    <t>tbl</t>
+  </si>
+  <si>
+    <t>Create a tibble data frame from a data source</t>
+  </si>
+  <si>
+    <t>show_query</t>
+  </si>
+  <si>
+    <t>Show the details of a tbl</t>
+  </si>
+  <si>
+    <t>dbplyr</t>
+  </si>
+  <si>
+    <t>dbExectute</t>
+  </si>
+  <si>
+    <t>Perform a database query</t>
+  </si>
+  <si>
+    <t>collect</t>
+  </si>
+  <si>
+    <t>Force computation of a database query</t>
+  </si>
+  <si>
+    <t>dbAppendTable</t>
+  </si>
+  <si>
+    <t>Modify an existing table in a database</t>
+  </si>
+  <si>
+    <t>dbDisconnect</t>
+  </si>
+  <si>
+    <t>Close the connection with a database</t>
+  </si>
+  <si>
+    <t>data.table</t>
+  </si>
+  <si>
+    <t>fread</t>
+  </si>
+  <si>
+    <t>Read in an object as a data.table class object</t>
+  </si>
+  <si>
+    <t>dtplyr</t>
+  </si>
+  <si>
+    <t>lazy_dt</t>
+  </si>
+  <si>
+    <t>Create a "lazy" data.table object that can be used with dplyr verbs</t>
+  </si>
+  <si>
+    <t>arrow</t>
+  </si>
+  <si>
+    <t>open_csv_dataset</t>
+  </si>
+  <si>
+    <t>Establish a connection with a csv data file</t>
   </si>
 </sst>
 </file>
@@ -2872,10 +2998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26B7B1B-D76F-6446-A51A-BD765778C143}">
-  <dimension ref="A1:D313"/>
+  <dimension ref="A1:D330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+    <sheetView tabSelected="1" topLeftCell="A179" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3615,16 +3741,16 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>703</v>
       </c>
       <c r="B53" t="s">
-        <v>186</v>
+        <v>704</v>
       </c>
       <c r="C53" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D53" t="s">
-        <v>187</v>
+        <v>705</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -3632,13 +3758,13 @@
         <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>449</v>
+        <v>186</v>
       </c>
       <c r="C54" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D54" t="s">
-        <v>450</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -3646,13 +3772,13 @@
         <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>190</v>
+        <v>449</v>
       </c>
       <c r="C55" t="s">
         <v>418</v>
       </c>
       <c r="D55" t="s">
-        <v>191</v>
+        <v>450</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -3660,13 +3786,13 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C56" t="s">
         <v>418</v>
       </c>
       <c r="D56" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -3674,13 +3800,13 @@
         <v>62</v>
       </c>
       <c r="B57" t="s">
-        <v>582</v>
+        <v>192</v>
       </c>
       <c r="C57" t="s">
         <v>418</v>
       </c>
       <c r="D57" t="s">
-        <v>583</v>
+        <v>193</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -3688,13 +3814,13 @@
         <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>607</v>
+        <v>582</v>
       </c>
       <c r="C58" t="s">
         <v>418</v>
       </c>
       <c r="D58" t="s">
-        <v>639</v>
+        <v>583</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -3702,13 +3828,13 @@
         <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
+        <v>607</v>
       </c>
       <c r="C59" t="s">
         <v>418</v>
       </c>
       <c r="D59" t="s">
-        <v>195</v>
+        <v>639</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -3716,13 +3842,13 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C60" t="s">
         <v>418</v>
       </c>
       <c r="D60" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -3730,13 +3856,13 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>483</v>
+        <v>196</v>
       </c>
       <c r="C61" t="s">
         <v>418</v>
       </c>
       <c r="D61" t="s">
-        <v>491</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -3744,13 +3870,13 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>198</v>
+        <v>483</v>
       </c>
       <c r="C62" t="s">
         <v>418</v>
       </c>
       <c r="D62" t="s">
-        <v>199</v>
+        <v>491</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -3758,13 +3884,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C63" t="s">
         <v>418</v>
       </c>
       <c r="D63" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -3772,13 +3898,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>63</v>
+        <v>200</v>
       </c>
       <c r="C64" t="s">
         <v>418</v>
       </c>
       <c r="D64" t="s">
-        <v>64</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -3786,13 +3912,13 @@
         <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>202</v>
+        <v>63</v>
       </c>
       <c r="C65" t="s">
         <v>418</v>
       </c>
       <c r="D65" t="s">
-        <v>203</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -3800,13 +3926,13 @@
         <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>65</v>
+        <v>202</v>
       </c>
       <c r="C66" t="s">
         <v>418</v>
       </c>
       <c r="D66" t="s">
-        <v>66</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -3814,13 +3940,13 @@
         <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>65</v>
       </c>
       <c r="C67" t="s">
         <v>418</v>
       </c>
       <c r="D67" t="s">
-        <v>205</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -3828,13 +3954,13 @@
         <v>62</v>
       </c>
       <c r="B68" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C68" t="s">
         <v>418</v>
       </c>
       <c r="D68" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -3842,13 +3968,13 @@
         <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C69" t="s">
         <v>418</v>
       </c>
       <c r="D69" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -3856,13 +3982,13 @@
         <v>62</v>
       </c>
       <c r="B70" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C70" t="s">
         <v>418</v>
       </c>
       <c r="D70" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -3870,13 +3996,13 @@
         <v>62</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>210</v>
       </c>
       <c r="C71" t="s">
         <v>418</v>
       </c>
       <c r="D71" t="s">
-        <v>68</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -3884,13 +4010,13 @@
         <v>62</v>
       </c>
       <c r="B72" t="s">
-        <v>212</v>
+        <v>67</v>
       </c>
       <c r="C72" t="s">
         <v>418</v>
       </c>
       <c r="D72" t="s">
-        <v>213</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -3898,13 +4024,13 @@
         <v>62</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>212</v>
       </c>
       <c r="C73" t="s">
         <v>418</v>
       </c>
       <c r="D73" t="s">
-        <v>70</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -3912,13 +4038,13 @@
         <v>62</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
         <v>418</v>
       </c>
       <c r="D74" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -3926,13 +4052,13 @@
         <v>62</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
         <v>418</v>
       </c>
       <c r="D75" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -3940,13 +4066,13 @@
         <v>62</v>
       </c>
       <c r="B76" t="s">
-        <v>214</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
         <v>418</v>
       </c>
       <c r="D76" t="s">
-        <v>215</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -3954,13 +4080,13 @@
         <v>62</v>
       </c>
       <c r="B77" t="s">
-        <v>559</v>
+        <v>214</v>
       </c>
       <c r="C77" t="s">
         <v>418</v>
       </c>
       <c r="D77" t="s">
-        <v>560</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -3968,13 +4094,13 @@
         <v>62</v>
       </c>
       <c r="B78" t="s">
-        <v>75</v>
+        <v>559</v>
       </c>
       <c r="C78" t="s">
         <v>418</v>
       </c>
       <c r="D78" t="s">
-        <v>76</v>
+        <v>560</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -3982,13 +4108,13 @@
         <v>62</v>
       </c>
       <c r="B79" t="s">
-        <v>216</v>
+        <v>75</v>
       </c>
       <c r="C79" t="s">
         <v>418</v>
       </c>
       <c r="D79" t="s">
-        <v>217</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -3996,13 +4122,13 @@
         <v>62</v>
       </c>
       <c r="B80" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C80" t="s">
         <v>418</v>
       </c>
       <c r="D80" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -4010,13 +4136,13 @@
         <v>62</v>
       </c>
       <c r="B81" t="s">
-        <v>470</v>
+        <v>218</v>
       </c>
       <c r="C81" t="s">
         <v>418</v>
       </c>
       <c r="D81" t="s">
-        <v>471</v>
+        <v>219</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -4024,13 +4150,13 @@
         <v>62</v>
       </c>
       <c r="B82" t="s">
-        <v>220</v>
+        <v>470</v>
       </c>
       <c r="C82" t="s">
         <v>418</v>
       </c>
       <c r="D82" t="s">
-        <v>221</v>
+        <v>471</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -4038,13 +4164,13 @@
         <v>62</v>
       </c>
       <c r="B83" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C83" t="s">
         <v>418</v>
       </c>
       <c r="D83" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -4052,13 +4178,13 @@
         <v>62</v>
       </c>
       <c r="B84" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C84" t="s">
         <v>418</v>
       </c>
       <c r="D84" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -4066,13 +4192,13 @@
         <v>62</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>224</v>
       </c>
       <c r="C85" t="s">
         <v>418</v>
       </c>
       <c r="D85" t="s">
-        <v>78</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -4080,139 +4206,139 @@
         <v>62</v>
       </c>
       <c r="B86" t="s">
-        <v>226</v>
+        <v>77</v>
       </c>
       <c r="C86" t="s">
         <v>418</v>
       </c>
       <c r="D86" t="s">
-        <v>227</v>
+        <v>78</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B87" t="s">
-        <v>80</v>
+        <v>226</v>
       </c>
       <c r="C87" t="s">
         <v>418</v>
       </c>
       <c r="D87" t="s">
-        <v>81</v>
+        <v>227</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B88" t="s">
-        <v>228</v>
+        <v>80</v>
       </c>
       <c r="C88" t="s">
         <v>418</v>
       </c>
       <c r="D88" t="s">
-        <v>229</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>82</v>
+        <v>697</v>
       </c>
       <c r="B89" t="s">
-        <v>230</v>
+        <v>698</v>
       </c>
       <c r="C89" t="s">
         <v>418</v>
       </c>
       <c r="D89" t="s">
-        <v>231</v>
+        <v>699</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>673</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>693</v>
       </c>
       <c r="C90" t="s">
         <v>418</v>
       </c>
       <c r="D90" t="s">
-        <v>84</v>
+        <v>694</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>82</v>
+        <v>673</v>
       </c>
       <c r="B91" t="s">
-        <v>232</v>
+        <v>674</v>
       </c>
       <c r="C91" t="s">
         <v>418</v>
       </c>
       <c r="D91" t="s">
-        <v>233</v>
+        <v>675</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>82</v>
+        <v>673</v>
       </c>
       <c r="B92" t="s">
-        <v>85</v>
+        <v>695</v>
       </c>
       <c r="C92" t="s">
         <v>418</v>
       </c>
       <c r="D92" t="s">
-        <v>86</v>
+        <v>696</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>82</v>
+        <v>673</v>
       </c>
       <c r="B93" t="s">
-        <v>576</v>
+        <v>681</v>
       </c>
       <c r="C93" t="s">
         <v>418</v>
       </c>
       <c r="D93" t="s">
-        <v>577</v>
+        <v>682</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>82</v>
+        <v>673</v>
       </c>
       <c r="B94" t="s">
-        <v>234</v>
+        <v>679</v>
       </c>
       <c r="C94" t="s">
         <v>418</v>
       </c>
       <c r="D94" t="s">
-        <v>235</v>
+        <v>680</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>82</v>
+        <v>688</v>
       </c>
       <c r="B95" t="s">
-        <v>236</v>
+        <v>689</v>
       </c>
       <c r="C95" t="s">
         <v>418</v>
       </c>
       <c r="D95" t="s">
-        <v>237</v>
+        <v>690</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -4220,13 +4346,13 @@
         <v>82</v>
       </c>
       <c r="B96" t="s">
-        <v>87</v>
+        <v>228</v>
       </c>
       <c r="C96" t="s">
         <v>418</v>
       </c>
       <c r="D96" t="s">
-        <v>88</v>
+        <v>229</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -4234,13 +4360,13 @@
         <v>82</v>
       </c>
       <c r="B97" t="s">
-        <v>89</v>
+        <v>230</v>
       </c>
       <c r="C97" t="s">
         <v>418</v>
       </c>
       <c r="D97" t="s">
-        <v>90</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -4248,27 +4374,27 @@
         <v>82</v>
       </c>
       <c r="B98" t="s">
-        <v>238</v>
+        <v>83</v>
       </c>
       <c r="C98" t="s">
         <v>418</v>
       </c>
       <c r="D98" t="s">
-        <v>239</v>
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="B99" t="s">
-        <v>124</v>
+        <v>232</v>
       </c>
       <c r="C99" t="s">
         <v>418</v>
       </c>
       <c r="D99" t="s">
-        <v>125</v>
+        <v>233</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -4276,13 +4402,13 @@
         <v>82</v>
       </c>
       <c r="B100" t="s">
-        <v>240</v>
+        <v>85</v>
       </c>
       <c r="C100" t="s">
         <v>418</v>
       </c>
       <c r="D100" t="s">
-        <v>241</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -4290,13 +4416,13 @@
         <v>82</v>
       </c>
       <c r="B101" t="s">
-        <v>242</v>
+        <v>576</v>
       </c>
       <c r="C101" t="s">
         <v>418</v>
       </c>
       <c r="D101" t="s">
-        <v>243</v>
+        <v>577</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -4304,13 +4430,13 @@
         <v>82</v>
       </c>
       <c r="B102" t="s">
-        <v>244</v>
+        <v>691</v>
       </c>
       <c r="C102" t="s">
         <v>418</v>
       </c>
       <c r="D102" t="s">
-        <v>245</v>
+        <v>692</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -4318,13 +4444,13 @@
         <v>82</v>
       </c>
       <c r="B103" t="s">
-        <v>91</v>
+        <v>234</v>
       </c>
       <c r="C103" t="s">
         <v>418</v>
       </c>
       <c r="D103" t="s">
-        <v>92</v>
+        <v>235</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -4332,13 +4458,13 @@
         <v>82</v>
       </c>
       <c r="B104" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C104" t="s">
         <v>418</v>
       </c>
       <c r="D104" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -4346,13 +4472,13 @@
         <v>82</v>
       </c>
       <c r="B105" t="s">
-        <v>248</v>
+        <v>87</v>
       </c>
       <c r="C105" t="s">
         <v>418</v>
       </c>
       <c r="D105" t="s">
-        <v>249</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -4360,13 +4486,13 @@
         <v>82</v>
       </c>
       <c r="B106" t="s">
-        <v>250</v>
+        <v>89</v>
       </c>
       <c r="C106" t="s">
         <v>418</v>
       </c>
       <c r="D106" t="s">
-        <v>251</v>
+        <v>90</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -4374,27 +4500,27 @@
         <v>82</v>
       </c>
       <c r="B107" t="s">
-        <v>93</v>
+        <v>238</v>
       </c>
       <c r="C107" t="s">
         <v>418</v>
       </c>
       <c r="D107" t="s">
-        <v>94</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="B108" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C108" t="s">
         <v>418</v>
       </c>
       <c r="D108" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -4402,13 +4528,13 @@
         <v>82</v>
       </c>
       <c r="B109" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C109" t="s">
         <v>418</v>
       </c>
       <c r="D109" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -4416,13 +4542,13 @@
         <v>82</v>
       </c>
       <c r="B110" t="s">
-        <v>97</v>
+        <v>242</v>
       </c>
       <c r="C110" t="s">
         <v>418</v>
       </c>
       <c r="D110" t="s">
-        <v>98</v>
+        <v>243</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -4430,13 +4556,13 @@
         <v>82</v>
       </c>
       <c r="B111" t="s">
-        <v>99</v>
+        <v>244</v>
       </c>
       <c r="C111" t="s">
         <v>418</v>
       </c>
       <c r="D111" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -4444,13 +4570,13 @@
         <v>82</v>
       </c>
       <c r="B112" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C112" t="s">
         <v>418</v>
       </c>
       <c r="D112" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -4458,13 +4584,13 @@
         <v>82</v>
       </c>
       <c r="B113" t="s">
-        <v>103</v>
+        <v>246</v>
       </c>
       <c r="C113" t="s">
         <v>418</v>
       </c>
       <c r="D113" t="s">
-        <v>416</v>
+        <v>247</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -4472,13 +4598,13 @@
         <v>82</v>
       </c>
       <c r="B114" t="s">
-        <v>104</v>
+        <v>248</v>
       </c>
       <c r="C114" t="s">
         <v>418</v>
       </c>
       <c r="D114" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -4486,13 +4612,13 @@
         <v>82</v>
       </c>
       <c r="B115" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C115" t="s">
         <v>418</v>
       </c>
       <c r="D115" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -4500,13 +4626,13 @@
         <v>82</v>
       </c>
       <c r="B116" t="s">
-        <v>256</v>
+        <v>93</v>
       </c>
       <c r="C116" t="s">
         <v>418</v>
       </c>
       <c r="D116" t="s">
-        <v>257</v>
+        <v>94</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -4514,13 +4640,13 @@
         <v>82</v>
       </c>
       <c r="B117" t="s">
-        <v>258</v>
+        <v>95</v>
       </c>
       <c r="C117" t="s">
         <v>418</v>
       </c>
       <c r="D117" t="s">
-        <v>259</v>
+        <v>96</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -4528,13 +4654,13 @@
         <v>82</v>
       </c>
       <c r="B118" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C118" t="s">
         <v>418</v>
       </c>
       <c r="D118" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -4542,13 +4668,13 @@
         <v>82</v>
       </c>
       <c r="B119" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C119" t="s">
         <v>418</v>
       </c>
       <c r="D119" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -4556,13 +4682,13 @@
         <v>82</v>
       </c>
       <c r="B120" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C120" t="s">
         <v>418</v>
       </c>
       <c r="D120" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -4570,13 +4696,13 @@
         <v>82</v>
       </c>
       <c r="B121" t="s">
-        <v>262</v>
+        <v>101</v>
       </c>
       <c r="C121" t="s">
         <v>418</v>
       </c>
       <c r="D121" t="s">
-        <v>263</v>
+        <v>102</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -4584,251 +4710,251 @@
         <v>82</v>
       </c>
       <c r="B122" t="s">
-        <v>264</v>
+        <v>103</v>
       </c>
       <c r="C122" t="s">
         <v>418</v>
       </c>
       <c r="D122" t="s">
-        <v>265</v>
+        <v>416</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>266</v>
+        <v>82</v>
       </c>
       <c r="B123" t="s">
-        <v>267</v>
+        <v>104</v>
       </c>
       <c r="C123" t="s">
         <v>418</v>
       </c>
       <c r="D123" t="s">
-        <v>268</v>
+        <v>105</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>266</v>
+        <v>82</v>
       </c>
       <c r="B124" t="s">
-        <v>269</v>
+        <v>686</v>
       </c>
       <c r="C124" t="s">
         <v>418</v>
       </c>
       <c r="D124" t="s">
-        <v>270</v>
+        <v>687</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>266</v>
+        <v>82</v>
       </c>
       <c r="B125" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="C125" t="s">
         <v>418</v>
       </c>
       <c r="D125" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>266</v>
+        <v>82</v>
       </c>
       <c r="B126" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="C126" t="s">
         <v>418</v>
       </c>
       <c r="D126" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>266</v>
+        <v>82</v>
       </c>
       <c r="B127" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C127" t="s">
         <v>418</v>
       </c>
       <c r="D127" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>277</v>
+        <v>82</v>
       </c>
       <c r="B128" t="s">
-        <v>10</v>
+        <v>260</v>
       </c>
       <c r="C128" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D128" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>277</v>
+        <v>82</v>
       </c>
       <c r="B129" t="s">
-        <v>279</v>
+        <v>106</v>
       </c>
       <c r="C129" t="s">
         <v>418</v>
       </c>
       <c r="D129" t="s">
-        <v>280</v>
+        <v>107</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>277</v>
+        <v>82</v>
       </c>
       <c r="B130" t="s">
-        <v>281</v>
+        <v>108</v>
       </c>
       <c r="C130" t="s">
         <v>418</v>
       </c>
       <c r="D130" t="s">
-        <v>282</v>
+        <v>109</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>277</v>
+        <v>683</v>
       </c>
       <c r="B131" t="s">
-        <v>283</v>
+        <v>684</v>
       </c>
       <c r="C131" t="s">
         <v>418</v>
       </c>
       <c r="D131" t="s">
-        <v>284</v>
+        <v>685</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>277</v>
+        <v>82</v>
       </c>
       <c r="B132" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="C132" t="s">
         <v>418</v>
       </c>
       <c r="D132" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>277</v>
+        <v>82</v>
       </c>
       <c r="B133" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="C133" t="s">
         <v>418</v>
       </c>
       <c r="D133" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>277</v>
+        <v>700</v>
       </c>
       <c r="B134" t="s">
-        <v>289</v>
+        <v>701</v>
       </c>
       <c r="C134" t="s">
         <v>418</v>
       </c>
       <c r="D134" t="s">
-        <v>290</v>
+        <v>702</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B135" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="C135" t="s">
         <v>418</v>
       </c>
       <c r="D135" t="s">
-        <v>663</v>
+        <v>268</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B136" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="C136" t="s">
         <v>418</v>
       </c>
       <c r="D136" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B137" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="C137" t="s">
         <v>418</v>
       </c>
       <c r="D137" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B138" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="C138" t="s">
         <v>418</v>
       </c>
       <c r="D138" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B139" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="C139" t="s">
         <v>418</v>
       </c>
       <c r="D139" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -4836,13 +4962,13 @@
         <v>277</v>
       </c>
       <c r="B140" t="s">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="C140" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D140" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -4850,13 +4976,13 @@
         <v>277</v>
       </c>
       <c r="B141" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="C141" t="s">
         <v>418</v>
       </c>
       <c r="D141" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -4864,13 +4990,13 @@
         <v>277</v>
       </c>
       <c r="B142" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="C142" t="s">
         <v>418</v>
       </c>
       <c r="D142" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -4878,13 +5004,13 @@
         <v>277</v>
       </c>
       <c r="B143" t="s">
-        <v>447</v>
+        <v>283</v>
       </c>
       <c r="C143" t="s">
         <v>418</v>
       </c>
       <c r="D143" t="s">
-        <v>448</v>
+        <v>284</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -4892,13 +5018,13 @@
         <v>277</v>
       </c>
       <c r="B144" t="s">
-        <v>459</v>
+        <v>285</v>
       </c>
       <c r="C144" t="s">
         <v>418</v>
       </c>
       <c r="D144" t="s">
-        <v>460</v>
+        <v>286</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -4906,13 +5032,13 @@
         <v>277</v>
       </c>
       <c r="B145" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="C145" t="s">
         <v>418</v>
       </c>
       <c r="D145" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -4920,13 +5046,13 @@
         <v>277</v>
       </c>
       <c r="B146" t="s">
-        <v>446</v>
+        <v>289</v>
       </c>
       <c r="C146" t="s">
         <v>418</v>
       </c>
       <c r="D146" t="s">
-        <v>461</v>
+        <v>290</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -4934,13 +5060,13 @@
         <v>277</v>
       </c>
       <c r="B147" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="C147" t="s">
         <v>418</v>
       </c>
       <c r="D147" t="s">
-        <v>309</v>
+        <v>663</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -4948,13 +5074,13 @@
         <v>277</v>
       </c>
       <c r="B148" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="C148" t="s">
         <v>418</v>
       </c>
       <c r="D148" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -4962,13 +5088,13 @@
         <v>277</v>
       </c>
       <c r="B149" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="C149" t="s">
         <v>418</v>
       </c>
       <c r="D149" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -4976,13 +5102,13 @@
         <v>277</v>
       </c>
       <c r="B150" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="C150" t="s">
         <v>418</v>
       </c>
       <c r="D150" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -4990,13 +5116,13 @@
         <v>277</v>
       </c>
       <c r="B151" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="C151" t="s">
         <v>418</v>
       </c>
       <c r="D151" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -5004,13 +5130,13 @@
         <v>277</v>
       </c>
       <c r="B152" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="C152" t="s">
         <v>418</v>
       </c>
       <c r="D152" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -5018,13 +5144,13 @@
         <v>277</v>
       </c>
       <c r="B153" t="s">
-        <v>462</v>
+        <v>302</v>
       </c>
       <c r="C153" t="s">
         <v>418</v>
       </c>
       <c r="D153" t="s">
-        <v>463</v>
+        <v>303</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -5032,13 +5158,13 @@
         <v>277</v>
       </c>
       <c r="B154" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="C154" t="s">
         <v>418</v>
       </c>
       <c r="D154" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -5046,13 +5172,13 @@
         <v>277</v>
       </c>
       <c r="B155" t="s">
-        <v>322</v>
+        <v>447</v>
       </c>
       <c r="C155" t="s">
         <v>418</v>
       </c>
       <c r="D155" t="s">
-        <v>323</v>
+        <v>448</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -5060,13 +5186,13 @@
         <v>277</v>
       </c>
       <c r="B156" t="s">
-        <v>324</v>
+        <v>459</v>
       </c>
       <c r="C156" t="s">
         <v>418</v>
       </c>
       <c r="D156" t="s">
-        <v>325</v>
+        <v>460</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -5074,13 +5200,13 @@
         <v>277</v>
       </c>
       <c r="B157" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="C157" t="s">
         <v>418</v>
       </c>
       <c r="D157" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -5088,13 +5214,13 @@
         <v>277</v>
       </c>
       <c r="B158" t="s">
-        <v>328</v>
+        <v>446</v>
       </c>
       <c r="C158" t="s">
         <v>418</v>
       </c>
       <c r="D158" t="s">
-        <v>329</v>
+        <v>461</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -5102,13 +5228,13 @@
         <v>277</v>
       </c>
       <c r="B159" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
       <c r="C159" t="s">
         <v>418</v>
       </c>
       <c r="D159" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -5116,13 +5242,13 @@
         <v>277</v>
       </c>
       <c r="B160" t="s">
-        <v>442</v>
+        <v>310</v>
       </c>
       <c r="C160" t="s">
         <v>418</v>
       </c>
       <c r="D160" t="s">
-        <v>443</v>
+        <v>311</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -5130,797 +5256,797 @@
         <v>277</v>
       </c>
       <c r="B161" t="s">
-        <v>445</v>
+        <v>312</v>
       </c>
       <c r="C161" t="s">
         <v>418</v>
       </c>
       <c r="D161" t="s">
-        <v>444</v>
+        <v>313</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>597</v>
+        <v>277</v>
       </c>
       <c r="B162" t="s">
-        <v>598</v>
+        <v>314</v>
       </c>
       <c r="C162" t="s">
         <v>418</v>
       </c>
       <c r="D162" t="s">
-        <v>599</v>
+        <v>315</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>611</v>
+        <v>277</v>
       </c>
       <c r="B163" t="s">
-        <v>612</v>
+        <v>316</v>
       </c>
       <c r="C163" t="s">
         <v>418</v>
       </c>
       <c r="D163" t="s">
-        <v>640</v>
+        <v>317</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>611</v>
+        <v>277</v>
       </c>
       <c r="B164" t="s">
-        <v>633</v>
+        <v>318</v>
       </c>
       <c r="C164" t="s">
         <v>418</v>
       </c>
       <c r="D164" t="s">
-        <v>641</v>
+        <v>319</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>609</v>
+        <v>277</v>
       </c>
       <c r="B165" t="s">
-        <v>610</v>
+        <v>462</v>
       </c>
       <c r="C165" t="s">
         <v>418</v>
       </c>
       <c r="D165" t="s">
-        <v>642</v>
+        <v>463</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>609</v>
+        <v>277</v>
       </c>
       <c r="B166" t="s">
-        <v>634</v>
+        <v>320</v>
       </c>
       <c r="C166" t="s">
         <v>418</v>
       </c>
       <c r="D166" t="s">
-        <v>656</v>
+        <v>321</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>609</v>
+        <v>277</v>
       </c>
       <c r="B167" t="s">
-        <v>635</v>
+        <v>322</v>
       </c>
       <c r="C167" t="s">
         <v>418</v>
       </c>
       <c r="D167" t="s">
-        <v>643</v>
+        <v>323</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>332</v>
+        <v>277</v>
       </c>
       <c r="B168" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C168" t="s">
         <v>418</v>
       </c>
       <c r="D168" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>332</v>
+        <v>277</v>
       </c>
       <c r="B169" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C169" t="s">
         <v>418</v>
       </c>
       <c r="D169" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>110</v>
+        <v>277</v>
       </c>
       <c r="B170" t="s">
-        <v>111</v>
+        <v>328</v>
       </c>
       <c r="C170" t="s">
         <v>418</v>
       </c>
       <c r="D170" t="s">
-        <v>112</v>
+        <v>329</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>110</v>
+        <v>277</v>
       </c>
       <c r="B171" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C171" t="s">
         <v>418</v>
       </c>
       <c r="D171" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>113</v>
+        <v>277</v>
       </c>
       <c r="B172" t="s">
-        <v>114</v>
+        <v>442</v>
       </c>
       <c r="C172" t="s">
         <v>418</v>
       </c>
       <c r="D172" t="s">
-        <v>115</v>
+        <v>443</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>113</v>
+        <v>277</v>
       </c>
       <c r="B173" t="s">
-        <v>339</v>
+        <v>445</v>
       </c>
       <c r="C173" t="s">
         <v>418</v>
       </c>
       <c r="D173" t="s">
-        <v>340</v>
+        <v>444</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>113</v>
+        <v>597</v>
       </c>
       <c r="B174" t="s">
-        <v>116</v>
+        <v>598</v>
       </c>
       <c r="C174" t="s">
         <v>418</v>
       </c>
       <c r="D174" t="s">
-        <v>117</v>
+        <v>599</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>113</v>
+        <v>611</v>
       </c>
       <c r="B175" t="s">
-        <v>341</v>
+        <v>612</v>
       </c>
       <c r="C175" t="s">
         <v>418</v>
       </c>
       <c r="D175" t="s">
-        <v>342</v>
+        <v>640</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>113</v>
+        <v>611</v>
       </c>
       <c r="B176" t="s">
-        <v>118</v>
+        <v>633</v>
       </c>
       <c r="C176" t="s">
         <v>418</v>
       </c>
       <c r="D176" t="s">
-        <v>119</v>
+        <v>641</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>113</v>
+        <v>609</v>
       </c>
       <c r="B177" t="s">
-        <v>343</v>
+        <v>610</v>
       </c>
       <c r="C177" t="s">
         <v>418</v>
       </c>
       <c r="D177" t="s">
-        <v>344</v>
+        <v>642</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>113</v>
+        <v>609</v>
       </c>
       <c r="B178" t="s">
-        <v>345</v>
+        <v>634</v>
       </c>
       <c r="C178" t="s">
         <v>418</v>
       </c>
       <c r="D178" t="s">
-        <v>346</v>
+        <v>656</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>113</v>
+        <v>609</v>
       </c>
       <c r="B179" t="s">
-        <v>349</v>
+        <v>635</v>
       </c>
       <c r="C179" t="s">
         <v>418</v>
       </c>
       <c r="D179" t="s">
-        <v>350</v>
+        <v>643</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>113</v>
+        <v>332</v>
       </c>
       <c r="B180" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="C180" t="s">
         <v>418</v>
       </c>
       <c r="D180" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>120</v>
+        <v>332</v>
       </c>
       <c r="B181" t="s">
-        <v>121</v>
+        <v>335</v>
       </c>
       <c r="C181" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D181" t="s">
-        <v>122</v>
+        <v>336</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B182" t="s">
-        <v>351</v>
+        <v>111</v>
       </c>
       <c r="C182" t="s">
         <v>418</v>
       </c>
       <c r="D182" t="s">
-        <v>352</v>
+        <v>112</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>514</v>
+        <v>110</v>
       </c>
       <c r="B183" t="s">
-        <v>515</v>
+        <v>337</v>
       </c>
       <c r="C183" t="s">
         <v>418</v>
       </c>
       <c r="D183" t="s">
-        <v>516</v>
+        <v>338</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>604</v>
+        <v>113</v>
       </c>
       <c r="B184" t="s">
-        <v>605</v>
+        <v>114</v>
       </c>
       <c r="C184" t="s">
         <v>418</v>
       </c>
       <c r="D184" t="s">
-        <v>644</v>
+        <v>115</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B185" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="C185" t="s">
         <v>418</v>
       </c>
       <c r="D185" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B186" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C186" t="s">
         <v>418</v>
       </c>
       <c r="D186" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B187" t="s">
-        <v>487</v>
+        <v>341</v>
       </c>
       <c r="C187" t="s">
         <v>418</v>
       </c>
       <c r="D187" t="s">
-        <v>492</v>
+        <v>342</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B188" t="s">
-        <v>486</v>
+        <v>118</v>
       </c>
       <c r="C188" t="s">
         <v>418</v>
       </c>
       <c r="D188" t="s">
-        <v>493</v>
+        <v>119</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B189" t="s">
-        <v>484</v>
+        <v>343</v>
       </c>
       <c r="C189" t="s">
         <v>418</v>
       </c>
       <c r="D189" t="s">
-        <v>494</v>
+        <v>344</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B190" t="s">
-        <v>485</v>
+        <v>345</v>
       </c>
       <c r="C190" t="s">
         <v>418</v>
       </c>
       <c r="D190" t="s">
-        <v>495</v>
+        <v>346</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B191" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C191" t="s">
         <v>418</v>
       </c>
       <c r="D191" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B192" t="s">
-        <v>129</v>
+        <v>347</v>
       </c>
       <c r="C192" t="s">
         <v>418</v>
       </c>
       <c r="D192" t="s">
-        <v>130</v>
+        <v>348</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>357</v>
+        <v>120</v>
       </c>
       <c r="B193" t="s">
-        <v>358</v>
+        <v>121</v>
       </c>
       <c r="C193" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D193" t="s">
-        <v>359</v>
+        <v>122</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B194" t="s">
-        <v>132</v>
+        <v>351</v>
       </c>
       <c r="C194" t="s">
         <v>418</v>
       </c>
       <c r="D194" t="s">
-        <v>133</v>
+        <v>352</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>131</v>
+        <v>514</v>
       </c>
       <c r="B195" t="s">
-        <v>360</v>
+        <v>515</v>
       </c>
       <c r="C195" t="s">
         <v>418</v>
       </c>
       <c r="D195" t="s">
-        <v>361</v>
+        <v>516</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>131</v>
+        <v>604</v>
       </c>
       <c r="B196" t="s">
-        <v>134</v>
+        <v>605</v>
       </c>
       <c r="C196" t="s">
         <v>418</v>
       </c>
       <c r="D196" t="s">
-        <v>135</v>
+        <v>644</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B197" t="s">
-        <v>136</v>
+        <v>353</v>
       </c>
       <c r="C197" t="s">
         <v>418</v>
       </c>
       <c r="D197" t="s">
-        <v>137</v>
+        <v>354</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B198" t="s">
-        <v>362</v>
+        <v>127</v>
       </c>
       <c r="C198" t="s">
         <v>418</v>
       </c>
       <c r="D198" t="s">
-        <v>363</v>
+        <v>128</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B199" t="s">
-        <v>138</v>
+        <v>487</v>
       </c>
       <c r="C199" t="s">
         <v>418</v>
       </c>
       <c r="D199" t="s">
-        <v>575</v>
+        <v>492</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>364</v>
+        <v>126</v>
       </c>
       <c r="B200" t="s">
-        <v>365</v>
+        <v>486</v>
       </c>
       <c r="C200" t="s">
         <v>418</v>
       </c>
       <c r="D200" t="s">
-        <v>366</v>
+        <v>493</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>364</v>
+        <v>126</v>
       </c>
       <c r="B201" t="s">
-        <v>367</v>
+        <v>484</v>
       </c>
       <c r="C201" t="s">
         <v>418</v>
       </c>
       <c r="D201" t="s">
-        <v>368</v>
+        <v>494</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B202" t="s">
-        <v>142</v>
+        <v>485</v>
       </c>
       <c r="C202" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D202" t="s">
-        <v>143</v>
+        <v>495</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B203" t="s">
-        <v>140</v>
+        <v>355</v>
       </c>
       <c r="C203" t="s">
         <v>418</v>
       </c>
       <c r="D203" t="s">
-        <v>141</v>
+        <v>356</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>521</v>
+        <v>126</v>
       </c>
       <c r="B204" t="s">
-        <v>522</v>
+        <v>129</v>
       </c>
       <c r="C204" t="s">
         <v>418</v>
       </c>
       <c r="D204" t="s">
-        <v>523</v>
+        <v>130</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>421</v>
+        <v>357</v>
       </c>
       <c r="B205" t="s">
-        <v>546</v>
+        <v>358</v>
       </c>
       <c r="C205" t="s">
         <v>418</v>
       </c>
       <c r="D205" t="s">
-        <v>570</v>
+        <v>359</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>421</v>
+        <v>131</v>
       </c>
       <c r="B206" t="s">
-        <v>422</v>
+        <v>132</v>
       </c>
       <c r="C206" t="s">
         <v>418</v>
       </c>
       <c r="D206" t="s">
-        <v>432</v>
+        <v>133</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>421</v>
+        <v>131</v>
       </c>
       <c r="B207" t="s">
-        <v>506</v>
+        <v>360</v>
       </c>
       <c r="C207" t="s">
         <v>418</v>
       </c>
       <c r="D207" t="s">
-        <v>507</v>
+        <v>361</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>421</v>
+        <v>131</v>
       </c>
       <c r="B208" t="s">
-        <v>524</v>
+        <v>134</v>
       </c>
       <c r="C208" t="s">
         <v>418</v>
       </c>
       <c r="D208" t="s">
-        <v>525</v>
+        <v>135</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>421</v>
+        <v>131</v>
       </c>
       <c r="B209" t="s">
-        <v>423</v>
+        <v>136</v>
       </c>
       <c r="C209" t="s">
         <v>418</v>
       </c>
       <c r="D209" t="s">
-        <v>433</v>
+        <v>137</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>421</v>
+        <v>131</v>
       </c>
       <c r="B210" t="s">
-        <v>547</v>
+        <v>362</v>
       </c>
       <c r="C210" t="s">
         <v>418</v>
       </c>
       <c r="D210" t="s">
-        <v>569</v>
+        <v>363</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>421</v>
+        <v>131</v>
       </c>
       <c r="B211" t="s">
-        <v>424</v>
+        <v>138</v>
       </c>
       <c r="C211" t="s">
         <v>418</v>
       </c>
       <c r="D211" t="s">
-        <v>434</v>
+        <v>575</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>421</v>
+        <v>364</v>
       </c>
       <c r="B212" t="s">
-        <v>548</v>
+        <v>365</v>
       </c>
       <c r="C212" t="s">
         <v>418</v>
       </c>
       <c r="D212" t="s">
-        <v>568</v>
+        <v>366</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>421</v>
+        <v>364</v>
       </c>
       <c r="B213" t="s">
-        <v>425</v>
+        <v>367</v>
       </c>
       <c r="C213" t="s">
         <v>418</v>
       </c>
       <c r="D213" t="s">
-        <v>435</v>
+        <v>368</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>421</v>
+        <v>139</v>
       </c>
       <c r="B214" t="s">
-        <v>549</v>
+        <v>142</v>
       </c>
       <c r="C214" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D214" t="s">
-        <v>571</v>
+        <v>143</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>421</v>
+        <v>139</v>
       </c>
       <c r="B215" t="s">
-        <v>453</v>
+        <v>140</v>
       </c>
       <c r="C215" t="s">
         <v>418</v>
       </c>
       <c r="D215" t="s">
-        <v>454</v>
+        <v>141</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>421</v>
+        <v>521</v>
       </c>
       <c r="B216" t="s">
-        <v>561</v>
+        <v>522</v>
       </c>
       <c r="C216" t="s">
         <v>418</v>
       </c>
       <c r="D216" t="s">
-        <v>572</v>
+        <v>523</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>421</v>
+        <v>676</v>
       </c>
       <c r="B217" t="s">
-        <v>550</v>
+        <v>677</v>
       </c>
       <c r="C217" t="s">
         <v>418</v>
       </c>
       <c r="D217" t="s">
-        <v>567</v>
+        <v>678</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
@@ -5928,13 +6054,13 @@
         <v>421</v>
       </c>
       <c r="B218" t="s">
-        <v>510</v>
+        <v>546</v>
       </c>
       <c r="C218" t="s">
         <v>418</v>
       </c>
       <c r="D218" t="s">
-        <v>511</v>
+        <v>570</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
@@ -5942,13 +6068,13 @@
         <v>421</v>
       </c>
       <c r="B219" t="s">
-        <v>464</v>
+        <v>422</v>
       </c>
       <c r="C219" t="s">
         <v>418</v>
       </c>
       <c r="D219" t="s">
-        <v>467</v>
+        <v>432</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
@@ -5956,13 +6082,13 @@
         <v>421</v>
       </c>
       <c r="B220" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="C220" t="s">
         <v>418</v>
       </c>
       <c r="D220" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
@@ -5970,13 +6096,13 @@
         <v>421</v>
       </c>
       <c r="B221" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
       <c r="C221" t="s">
         <v>418</v>
       </c>
       <c r="D221" t="s">
-        <v>573</v>
+        <v>525</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -5984,13 +6110,13 @@
         <v>421</v>
       </c>
       <c r="B222" t="s">
-        <v>468</v>
+        <v>423</v>
       </c>
       <c r="C222" t="s">
         <v>418</v>
       </c>
       <c r="D222" t="s">
-        <v>469</v>
+        <v>433</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -5998,13 +6124,13 @@
         <v>421</v>
       </c>
       <c r="B223" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C223" t="s">
         <v>418</v>
       </c>
       <c r="D223" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -6012,13 +6138,13 @@
         <v>421</v>
       </c>
       <c r="B224" t="s">
-        <v>465</v>
+        <v>424</v>
       </c>
       <c r="C224" t="s">
         <v>418</v>
       </c>
       <c r="D224" t="s">
-        <v>466</v>
+        <v>434</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -6026,13 +6152,13 @@
         <v>421</v>
       </c>
       <c r="B225" t="s">
-        <v>426</v>
+        <v>548</v>
       </c>
       <c r="C225" t="s">
         <v>418</v>
       </c>
       <c r="D225" t="s">
-        <v>436</v>
+        <v>568</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -6040,13 +6166,13 @@
         <v>421</v>
       </c>
       <c r="B226" t="s">
-        <v>552</v>
+        <v>425</v>
       </c>
       <c r="C226" t="s">
         <v>418</v>
       </c>
       <c r="D226" t="s">
-        <v>565</v>
+        <v>435</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -6054,13 +6180,13 @@
         <v>421</v>
       </c>
       <c r="B227" t="s">
-        <v>427</v>
+        <v>549</v>
       </c>
       <c r="C227" t="s">
         <v>418</v>
       </c>
       <c r="D227" t="s">
-        <v>437</v>
+        <v>571</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
@@ -6068,13 +6194,13 @@
         <v>421</v>
       </c>
       <c r="B228" t="s">
-        <v>428</v>
+        <v>453</v>
       </c>
       <c r="C228" t="s">
         <v>418</v>
       </c>
       <c r="D228" t="s">
-        <v>438</v>
+        <v>454</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
@@ -6082,13 +6208,13 @@
         <v>421</v>
       </c>
       <c r="B229" t="s">
-        <v>429</v>
+        <v>561</v>
       </c>
       <c r="C229" t="s">
         <v>418</v>
       </c>
       <c r="D229" t="s">
-        <v>439</v>
+        <v>572</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -6096,13 +6222,13 @@
         <v>421</v>
       </c>
       <c r="B230" t="s">
-        <v>630</v>
+        <v>550</v>
       </c>
       <c r="C230" t="s">
         <v>418</v>
       </c>
       <c r="D230" t="s">
-        <v>645</v>
+        <v>567</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
@@ -6110,13 +6236,13 @@
         <v>421</v>
       </c>
       <c r="B231" t="s">
-        <v>430</v>
+        <v>510</v>
       </c>
       <c r="C231" t="s">
         <v>418</v>
       </c>
       <c r="D231" t="s">
-        <v>440</v>
+        <v>511</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -6124,13 +6250,13 @@
         <v>421</v>
       </c>
       <c r="B232" t="s">
-        <v>431</v>
+        <v>464</v>
       </c>
       <c r="C232" t="s">
         <v>418</v>
       </c>
       <c r="D232" t="s">
-        <v>441</v>
+        <v>467</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
@@ -6138,13 +6264,13 @@
         <v>421</v>
       </c>
       <c r="B233" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="C233" t="s">
         <v>418</v>
       </c>
       <c r="D233" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -6152,13 +6278,13 @@
         <v>421</v>
       </c>
       <c r="B234" t="s">
-        <v>451</v>
+        <v>545</v>
       </c>
       <c r="C234" t="s">
         <v>418</v>
       </c>
       <c r="D234" t="s">
-        <v>452</v>
+        <v>573</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
@@ -6166,13 +6292,13 @@
         <v>421</v>
       </c>
       <c r="B235" t="s">
-        <v>517</v>
+        <v>468</v>
       </c>
       <c r="C235" t="s">
         <v>418</v>
       </c>
       <c r="D235" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
@@ -6180,531 +6306,531 @@
         <v>421</v>
       </c>
       <c r="B236" t="s">
-        <v>455</v>
+        <v>551</v>
       </c>
       <c r="C236" t="s">
         <v>418</v>
       </c>
       <c r="D236" t="s">
-        <v>456</v>
+        <v>566</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>602</v>
+        <v>421</v>
       </c>
       <c r="B237" t="s">
-        <v>603</v>
+        <v>465</v>
       </c>
       <c r="C237" t="s">
         <v>418</v>
       </c>
       <c r="D237" t="s">
-        <v>646</v>
+        <v>466</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>602</v>
+        <v>421</v>
       </c>
       <c r="B238" t="s">
-        <v>623</v>
+        <v>426</v>
       </c>
       <c r="C238" t="s">
         <v>418</v>
       </c>
       <c r="D238" t="s">
-        <v>647</v>
+        <v>436</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>615</v>
+        <v>421</v>
       </c>
       <c r="B239" t="s">
-        <v>616</v>
+        <v>552</v>
       </c>
       <c r="C239" t="s">
         <v>418</v>
       </c>
       <c r="D239" t="s">
-        <v>648</v>
+        <v>565</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>615</v>
+        <v>421</v>
       </c>
       <c r="B240" t="s">
-        <v>619</v>
+        <v>427</v>
       </c>
       <c r="C240" t="s">
         <v>418</v>
       </c>
       <c r="D240" t="s">
-        <v>649</v>
+        <v>437</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>620</v>
+        <v>421</v>
       </c>
       <c r="B241" t="s">
-        <v>621</v>
+        <v>428</v>
       </c>
       <c r="C241" t="s">
         <v>418</v>
       </c>
       <c r="D241" t="s">
-        <v>650</v>
+        <v>438</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>620</v>
+        <v>421</v>
       </c>
       <c r="B242" t="s">
-        <v>622</v>
+        <v>429</v>
       </c>
       <c r="C242" t="s">
         <v>418</v>
       </c>
       <c r="D242" t="s">
-        <v>651</v>
+        <v>439</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>628</v>
+        <v>421</v>
       </c>
       <c r="B243" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C243" t="s">
         <v>418</v>
       </c>
       <c r="D243" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>369</v>
+        <v>421</v>
       </c>
       <c r="B244" t="s">
-        <v>606</v>
+        <v>430</v>
       </c>
       <c r="C244" t="s">
         <v>418</v>
       </c>
       <c r="D244" t="s">
-        <v>653</v>
+        <v>440</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>369</v>
+        <v>421</v>
       </c>
       <c r="B245" t="s">
-        <v>614</v>
+        <v>431</v>
       </c>
       <c r="C245" t="s">
         <v>418</v>
       </c>
       <c r="D245" t="s">
-        <v>654</v>
+        <v>441</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>369</v>
+        <v>421</v>
       </c>
       <c r="B246" t="s">
-        <v>370</v>
+        <v>519</v>
       </c>
       <c r="C246" t="s">
         <v>418</v>
       </c>
       <c r="D246" t="s">
-        <v>371</v>
+        <v>520</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>369</v>
+        <v>421</v>
       </c>
       <c r="B247" t="s">
-        <v>584</v>
+        <v>451</v>
       </c>
       <c r="C247" t="s">
         <v>418</v>
       </c>
       <c r="D247" t="s">
-        <v>585</v>
+        <v>452</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>369</v>
+        <v>421</v>
       </c>
       <c r="B248" t="s">
-        <v>624</v>
+        <v>517</v>
       </c>
       <c r="C248" t="s">
         <v>418</v>
       </c>
       <c r="D248" t="s">
-        <v>655</v>
+        <v>518</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>369</v>
+        <v>421</v>
       </c>
       <c r="B249" t="s">
-        <v>372</v>
+        <v>455</v>
       </c>
       <c r="C249" t="s">
         <v>418</v>
       </c>
       <c r="D249" t="s">
-        <v>373</v>
+        <v>456</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>369</v>
+        <v>602</v>
       </c>
       <c r="B250" t="s">
-        <v>374</v>
+        <v>603</v>
       </c>
       <c r="C250" t="s">
         <v>418</v>
       </c>
       <c r="D250" t="s">
-        <v>419</v>
+        <v>646</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>369</v>
+        <v>602</v>
       </c>
       <c r="B251" t="s">
-        <v>588</v>
+        <v>623</v>
       </c>
       <c r="C251" t="s">
         <v>418</v>
       </c>
       <c r="D251" t="s">
-        <v>589</v>
+        <v>647</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>369</v>
+        <v>615</v>
       </c>
       <c r="B252" t="s">
-        <v>375</v>
+        <v>616</v>
       </c>
       <c r="C252" t="s">
         <v>418</v>
       </c>
       <c r="D252" t="s">
-        <v>376</v>
+        <v>648</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>144</v>
+        <v>615</v>
       </c>
       <c r="B253" t="s">
-        <v>145</v>
+        <v>619</v>
       </c>
       <c r="C253" t="s">
         <v>418</v>
       </c>
       <c r="D253" t="s">
-        <v>146</v>
+        <v>649</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>144</v>
+        <v>620</v>
       </c>
       <c r="B254" t="s">
-        <v>377</v>
+        <v>621</v>
       </c>
       <c r="C254" t="s">
         <v>418</v>
       </c>
       <c r="D254" t="s">
-        <v>378</v>
+        <v>650</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>144</v>
+        <v>620</v>
       </c>
       <c r="B255" t="s">
-        <v>590</v>
+        <v>622</v>
       </c>
       <c r="C255" t="s">
         <v>418</v>
       </c>
       <c r="D255" t="s">
-        <v>591</v>
+        <v>651</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>144</v>
+        <v>628</v>
       </c>
       <c r="B256" t="s">
-        <v>379</v>
+        <v>629</v>
       </c>
       <c r="C256" t="s">
         <v>418</v>
       </c>
       <c r="D256" t="s">
-        <v>380</v>
+        <v>652</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>144</v>
+        <v>369</v>
       </c>
       <c r="B257" t="s">
-        <v>381</v>
+        <v>606</v>
       </c>
       <c r="C257" t="s">
         <v>418</v>
       </c>
       <c r="D257" t="s">
-        <v>382</v>
+        <v>653</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>144</v>
+        <v>369</v>
       </c>
       <c r="B258" t="s">
-        <v>592</v>
+        <v>614</v>
       </c>
       <c r="C258" t="s">
         <v>418</v>
       </c>
       <c r="D258" t="s">
-        <v>594</v>
+        <v>654</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>144</v>
+        <v>369</v>
       </c>
       <c r="B259" t="s">
-        <v>593</v>
+        <v>370</v>
       </c>
       <c r="C259" t="s">
         <v>418</v>
       </c>
       <c r="D259" t="s">
-        <v>595</v>
+        <v>371</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>530</v>
+        <v>369</v>
       </c>
       <c r="B260" t="s">
-        <v>600</v>
+        <v>584</v>
       </c>
       <c r="C260" t="s">
         <v>418</v>
       </c>
       <c r="D260" t="s">
-        <v>601</v>
+        <v>585</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>530</v>
+        <v>369</v>
       </c>
       <c r="B261" t="s">
-        <v>578</v>
+        <v>624</v>
       </c>
       <c r="C261" t="s">
         <v>418</v>
       </c>
       <c r="D261" t="s">
-        <v>579</v>
+        <v>655</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>530</v>
+        <v>369</v>
       </c>
       <c r="B262" t="s">
-        <v>580</v>
+        <v>372</v>
       </c>
       <c r="C262" t="s">
         <v>418</v>
       </c>
       <c r="D262" t="s">
-        <v>581</v>
+        <v>373</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>530</v>
+        <v>369</v>
       </c>
       <c r="B263" t="s">
-        <v>531</v>
+        <v>374</v>
       </c>
       <c r="C263" t="s">
         <v>418</v>
       </c>
       <c r="D263" t="s">
-        <v>538</v>
+        <v>419</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>530</v>
+        <v>369</v>
       </c>
       <c r="B264" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="C264" t="s">
         <v>418</v>
       </c>
       <c r="D264" t="s">
-        <v>657</v>
+        <v>589</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>530</v>
+        <v>369</v>
       </c>
       <c r="B265" t="s">
-        <v>351</v>
+        <v>375</v>
       </c>
       <c r="C265" t="s">
         <v>418</v>
       </c>
       <c r="D265" t="s">
-        <v>596</v>
+        <v>376</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>530</v>
+        <v>668</v>
       </c>
       <c r="B266" t="s">
-        <v>532</v>
+        <v>669</v>
       </c>
       <c r="C266" t="s">
         <v>418</v>
       </c>
       <c r="D266" t="s">
-        <v>539</v>
+        <v>670</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B267" t="s">
-        <v>533</v>
+        <v>145</v>
       </c>
       <c r="C267" t="s">
         <v>418</v>
       </c>
       <c r="D267" t="s">
-        <v>540</v>
+        <v>146</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B268" t="s">
-        <v>534</v>
+        <v>377</v>
       </c>
       <c r="C268" t="s">
         <v>418</v>
       </c>
       <c r="D268" t="s">
-        <v>541</v>
+        <v>378</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B269" t="s">
-        <v>535</v>
+        <v>590</v>
       </c>
       <c r="C269" t="s">
         <v>418</v>
       </c>
       <c r="D269" t="s">
-        <v>542</v>
+        <v>591</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B270" t="s">
-        <v>536</v>
+        <v>379</v>
       </c>
       <c r="C270" t="s">
         <v>418</v>
       </c>
       <c r="D270" t="s">
-        <v>543</v>
+        <v>380</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B271" t="s">
-        <v>586</v>
+        <v>381</v>
       </c>
       <c r="C271" t="s">
         <v>418</v>
       </c>
       <c r="D271" t="s">
-        <v>587</v>
+        <v>382</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B272" t="s">
-        <v>625</v>
+        <v>592</v>
       </c>
       <c r="C272" t="s">
         <v>418</v>
       </c>
       <c r="D272" t="s">
-        <v>658</v>
+        <v>594</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B273" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="C273" t="s">
         <v>418</v>
       </c>
       <c r="D273" t="s">
-        <v>659</v>
+        <v>595</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
@@ -6712,13 +6838,13 @@
         <v>530</v>
       </c>
       <c r="B274" t="s">
-        <v>627</v>
+        <v>600</v>
       </c>
       <c r="C274" t="s">
         <v>418</v>
       </c>
       <c r="D274" t="s">
-        <v>660</v>
+        <v>601</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
@@ -6726,13 +6852,13 @@
         <v>530</v>
       </c>
       <c r="B275" t="s">
-        <v>632</v>
+        <v>578</v>
       </c>
       <c r="C275" t="s">
         <v>418</v>
       </c>
       <c r="D275" t="s">
-        <v>661</v>
+        <v>579</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
@@ -6740,530 +6866,768 @@
         <v>530</v>
       </c>
       <c r="B276" t="s">
-        <v>537</v>
+        <v>580</v>
       </c>
       <c r="C276" t="s">
         <v>418</v>
       </c>
       <c r="D276" t="s">
-        <v>544</v>
+        <v>581</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>147</v>
+        <v>530</v>
       </c>
       <c r="B277" t="s">
-        <v>457</v>
+        <v>531</v>
       </c>
       <c r="C277" t="s">
         <v>418</v>
       </c>
       <c r="D277" t="s">
-        <v>458</v>
+        <v>538</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>147</v>
+        <v>530</v>
       </c>
       <c r="B278" t="s">
-        <v>383</v>
+        <v>608</v>
       </c>
       <c r="C278" t="s">
         <v>418</v>
       </c>
       <c r="D278" t="s">
-        <v>384</v>
+        <v>657</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>147</v>
+        <v>530</v>
       </c>
       <c r="B279" t="s">
-        <v>147</v>
+        <v>351</v>
       </c>
       <c r="C279" t="s">
         <v>418</v>
       </c>
       <c r="D279" t="s">
-        <v>148</v>
+        <v>596</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>147</v>
+        <v>530</v>
       </c>
       <c r="B280" t="s">
-        <v>385</v>
+        <v>532</v>
       </c>
       <c r="C280" t="s">
         <v>418</v>
       </c>
       <c r="D280" t="s">
-        <v>386</v>
+        <v>539</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>149</v>
+        <v>530</v>
       </c>
       <c r="B281" t="s">
-        <v>387</v>
+        <v>533</v>
       </c>
       <c r="C281" t="s">
         <v>418</v>
       </c>
       <c r="D281" t="s">
-        <v>388</v>
+        <v>540</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>149</v>
+        <v>530</v>
       </c>
       <c r="B282" t="s">
-        <v>389</v>
+        <v>534</v>
       </c>
       <c r="C282" t="s">
         <v>418</v>
       </c>
       <c r="D282" t="s">
-        <v>390</v>
+        <v>541</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>149</v>
+        <v>530</v>
       </c>
       <c r="B283" t="s">
-        <v>391</v>
+        <v>535</v>
       </c>
       <c r="C283" t="s">
         <v>418</v>
       </c>
       <c r="D283" t="s">
-        <v>392</v>
+        <v>542</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>149</v>
+        <v>530</v>
       </c>
       <c r="B284" t="s">
-        <v>393</v>
+        <v>536</v>
       </c>
       <c r="C284" t="s">
         <v>418</v>
       </c>
       <c r="D284" t="s">
-        <v>394</v>
+        <v>543</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>149</v>
+        <v>530</v>
       </c>
       <c r="B285" t="s">
-        <v>395</v>
+        <v>586</v>
       </c>
       <c r="C285" t="s">
         <v>418</v>
       </c>
       <c r="D285" t="s">
-        <v>396</v>
+        <v>587</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>149</v>
+        <v>530</v>
       </c>
       <c r="B286" t="s">
-        <v>397</v>
+        <v>625</v>
       </c>
       <c r="C286" t="s">
         <v>418</v>
       </c>
       <c r="D286" t="s">
-        <v>398</v>
+        <v>658</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>473</v>
+        <v>530</v>
       </c>
       <c r="B287" t="s">
-        <v>482</v>
+        <v>626</v>
       </c>
       <c r="C287" t="s">
         <v>418</v>
       </c>
       <c r="D287" t="s">
-        <v>496</v>
+        <v>659</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>473</v>
+        <v>530</v>
       </c>
       <c r="B288" t="s">
-        <v>526</v>
+        <v>627</v>
       </c>
       <c r="C288" t="s">
         <v>418</v>
       </c>
       <c r="D288" t="s">
-        <v>527</v>
+        <v>660</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>473</v>
+        <v>530</v>
       </c>
       <c r="B289" t="s">
-        <v>480</v>
+        <v>632</v>
       </c>
       <c r="C289" t="s">
         <v>418</v>
       </c>
       <c r="D289" t="s">
-        <v>497</v>
+        <v>661</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>473</v>
+        <v>530</v>
       </c>
       <c r="B290" t="s">
-        <v>481</v>
+        <v>537</v>
       </c>
       <c r="C290" t="s">
         <v>418</v>
       </c>
       <c r="D290" t="s">
-        <v>498</v>
+        <v>544</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>473</v>
+        <v>147</v>
       </c>
       <c r="B291" t="s">
-        <v>476</v>
+        <v>457</v>
       </c>
       <c r="C291" t="s">
         <v>418</v>
       </c>
       <c r="D291" t="s">
-        <v>499</v>
+        <v>458</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>473</v>
+        <v>147</v>
       </c>
       <c r="B292" t="s">
-        <v>553</v>
+        <v>383</v>
       </c>
       <c r="C292" t="s">
         <v>418</v>
       </c>
       <c r="D292" t="s">
-        <v>562</v>
+        <v>384</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>473</v>
+        <v>147</v>
       </c>
       <c r="B293" t="s">
-        <v>504</v>
+        <v>147</v>
       </c>
       <c r="C293" t="s">
         <v>418</v>
       </c>
       <c r="D293" t="s">
-        <v>505</v>
+        <v>148</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>473</v>
+        <v>147</v>
       </c>
       <c r="B294" t="s">
-        <v>475</v>
+        <v>385</v>
       </c>
       <c r="C294" t="s">
         <v>418</v>
       </c>
       <c r="D294" t="s">
-        <v>500</v>
+        <v>386</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>473</v>
+        <v>149</v>
       </c>
       <c r="B295" t="s">
-        <v>508</v>
+        <v>387</v>
       </c>
       <c r="C295" t="s">
         <v>418</v>
       </c>
       <c r="D295" t="s">
-        <v>509</v>
+        <v>388</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>473</v>
+        <v>149</v>
       </c>
       <c r="B296" t="s">
-        <v>477</v>
+        <v>671</v>
       </c>
       <c r="C296" t="s">
         <v>418</v>
       </c>
       <c r="D296" t="s">
-        <v>501</v>
+        <v>672</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>473</v>
+        <v>149</v>
       </c>
       <c r="B297" t="s">
-        <v>474</v>
+        <v>664</v>
       </c>
       <c r="C297" t="s">
         <v>418</v>
       </c>
       <c r="D297" t="s">
-        <v>502</v>
+        <v>665</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>473</v>
+        <v>149</v>
       </c>
       <c r="B298" t="s">
-        <v>528</v>
+        <v>389</v>
       </c>
       <c r="C298" t="s">
         <v>418</v>
       </c>
       <c r="D298" t="s">
-        <v>529</v>
+        <v>390</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>478</v>
+        <v>149</v>
       </c>
       <c r="B299" t="s">
-        <v>479</v>
+        <v>391</v>
       </c>
       <c r="C299" t="s">
         <v>418</v>
       </c>
       <c r="D299" t="s">
-        <v>503</v>
+        <v>392</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>399</v>
+        <v>149</v>
       </c>
       <c r="B300" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="C300" t="s">
         <v>418</v>
       </c>
       <c r="D300" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>399</v>
+        <v>149</v>
       </c>
       <c r="B301" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C301" t="s">
         <v>418</v>
       </c>
       <c r="D301" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>399</v>
+        <v>149</v>
       </c>
       <c r="B302" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C302" t="s">
         <v>418</v>
       </c>
       <c r="D302" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>405</v>
+        <v>149</v>
       </c>
       <c r="B303" t="s">
-        <v>406</v>
+        <v>666</v>
       </c>
       <c r="C303" t="s">
         <v>418</v>
       </c>
       <c r="D303" t="s">
-        <v>407</v>
+        <v>667</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>405</v>
+        <v>473</v>
       </c>
       <c r="B304" t="s">
-        <v>408</v>
+        <v>482</v>
       </c>
       <c r="C304" t="s">
         <v>418</v>
       </c>
       <c r="D304" t="s">
-        <v>409</v>
+        <v>496</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>554</v>
+        <v>473</v>
       </c>
       <c r="B305" t="s">
-        <v>556</v>
+        <v>526</v>
       </c>
       <c r="C305" t="s">
         <v>418</v>
       </c>
       <c r="D305" t="s">
-        <v>563</v>
+        <v>527</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>554</v>
+        <v>473</v>
       </c>
       <c r="B306" t="s">
-        <v>555</v>
+        <v>480</v>
       </c>
       <c r="C306" t="s">
         <v>418</v>
       </c>
       <c r="D306" t="s">
-        <v>564</v>
+        <v>497</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>150</v>
+        <v>473</v>
       </c>
       <c r="B307" t="s">
-        <v>410</v>
+        <v>481</v>
       </c>
       <c r="C307" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D307" t="s">
-        <v>411</v>
+        <v>498</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>62</v>
+        <v>473</v>
       </c>
       <c r="B308" t="s">
-        <v>613</v>
+        <v>476</v>
       </c>
       <c r="C308" t="s">
         <v>418</v>
       </c>
       <c r="D308" t="s">
-        <v>637</v>
+        <v>499</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>150</v>
+        <v>473</v>
       </c>
       <c r="B309" t="s">
-        <v>151</v>
+        <v>553</v>
       </c>
       <c r="C309" t="s">
         <v>418</v>
       </c>
       <c r="D309" t="s">
-        <v>662</v>
+        <v>562</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>150</v>
+        <v>473</v>
       </c>
       <c r="B310" t="s">
-        <v>412</v>
+        <v>504</v>
       </c>
       <c r="C310" t="s">
         <v>418</v>
       </c>
       <c r="D310" t="s">
-        <v>413</v>
+        <v>505</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>150</v>
+        <v>473</v>
       </c>
       <c r="B311" t="s">
-        <v>557</v>
+        <v>475</v>
       </c>
       <c r="C311" t="s">
         <v>418</v>
       </c>
       <c r="D311" t="s">
-        <v>558</v>
+        <v>500</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>150</v>
+        <v>473</v>
       </c>
       <c r="B312" t="s">
-        <v>152</v>
+        <v>508</v>
       </c>
       <c r="C312" t="s">
         <v>418</v>
       </c>
       <c r="D312" t="s">
-        <v>153</v>
+        <v>509</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
+        <v>473</v>
+      </c>
+      <c r="B313" t="s">
+        <v>477</v>
+      </c>
+      <c r="C313" t="s">
+        <v>418</v>
+      </c>
+      <c r="D313" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>473</v>
+      </c>
+      <c r="B314" t="s">
+        <v>474</v>
+      </c>
+      <c r="C314" t="s">
+        <v>418</v>
+      </c>
+      <c r="D314" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>473</v>
+      </c>
+      <c r="B315" t="s">
+        <v>528</v>
+      </c>
+      <c r="C315" t="s">
+        <v>418</v>
+      </c>
+      <c r="D315" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>478</v>
+      </c>
+      <c r="B316" t="s">
+        <v>479</v>
+      </c>
+      <c r="C316" t="s">
+        <v>418</v>
+      </c>
+      <c r="D316" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>399</v>
+      </c>
+      <c r="B317" t="s">
+        <v>400</v>
+      </c>
+      <c r="C317" t="s">
+        <v>418</v>
+      </c>
+      <c r="D317" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>399</v>
+      </c>
+      <c r="B318" t="s">
+        <v>401</v>
+      </c>
+      <c r="C318" t="s">
+        <v>418</v>
+      </c>
+      <c r="D318" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>399</v>
+      </c>
+      <c r="B319" t="s">
+        <v>403</v>
+      </c>
+      <c r="C319" t="s">
+        <v>418</v>
+      </c>
+      <c r="D319" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>405</v>
+      </c>
+      <c r="B320" t="s">
+        <v>406</v>
+      </c>
+      <c r="C320" t="s">
+        <v>418</v>
+      </c>
+      <c r="D320" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A321" t="s">
+        <v>405</v>
+      </c>
+      <c r="B321" t="s">
+        <v>408</v>
+      </c>
+      <c r="C321" t="s">
+        <v>418</v>
+      </c>
+      <c r="D321" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A322" t="s">
+        <v>554</v>
+      </c>
+      <c r="B322" t="s">
+        <v>556</v>
+      </c>
+      <c r="C322" t="s">
+        <v>418</v>
+      </c>
+      <c r="D322" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A323" t="s">
+        <v>554</v>
+      </c>
+      <c r="B323" t="s">
+        <v>555</v>
+      </c>
+      <c r="C323" t="s">
+        <v>418</v>
+      </c>
+      <c r="D323" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A324" t="s">
         <v>150</v>
       </c>
-      <c r="B313" t="s">
+      <c r="B324" t="s">
+        <v>410</v>
+      </c>
+      <c r="C324" t="s">
+        <v>417</v>
+      </c>
+      <c r="D324" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
+        <v>62</v>
+      </c>
+      <c r="B325" t="s">
+        <v>613</v>
+      </c>
+      <c r="C325" t="s">
+        <v>418</v>
+      </c>
+      <c r="D325" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A326" t="s">
+        <v>150</v>
+      </c>
+      <c r="B326" t="s">
+        <v>151</v>
+      </c>
+      <c r="C326" t="s">
+        <v>418</v>
+      </c>
+      <c r="D326" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A327" t="s">
+        <v>150</v>
+      </c>
+      <c r="B327" t="s">
+        <v>412</v>
+      </c>
+      <c r="C327" t="s">
+        <v>418</v>
+      </c>
+      <c r="D327" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A328" t="s">
+        <v>150</v>
+      </c>
+      <c r="B328" t="s">
+        <v>557</v>
+      </c>
+      <c r="C328" t="s">
+        <v>418</v>
+      </c>
+      <c r="D328" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>150</v>
+      </c>
+      <c r="B329" t="s">
+        <v>152</v>
+      </c>
+      <c r="C329" t="s">
+        <v>418</v>
+      </c>
+      <c r="D329" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>150</v>
+      </c>
+      <c r="B330" t="s">
         <v>631</v>
       </c>
-      <c r="C313" t="s">
+      <c r="C330" t="s">
         <v>631</v>
       </c>
-      <c r="D313" t="s">
+      <c r="D330" t="s">
         <v>636</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added custom package functions
</commit_message>
<xml_diff>
--- a/big_functions_frame.xlsx
+++ b/big_functions_frame.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ssd980/datasci_2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarasnedgen/gits/datasci_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13010EA6-D917-AF41-A07B-317F63082857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D06517B-0879-BF40-ADD2-BDFB92363C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21600" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{95C4795D-FAAA-484B-ACF2-0B904DFB98DD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{95C4795D-FAAA-484B-ACF2-0B904DFB98DD}"/>
   </bookViews>
   <sheets>
     <sheet name="big_functions_frame" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="724">
   <si>
     <t>package</t>
   </si>
@@ -2138,6 +2138,60 @@
   </si>
   <si>
     <t>Establish a connection with a csv data file</t>
+  </si>
+  <si>
+    <t>devtools</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>install</t>
+  </si>
+  <si>
+    <t>load_all</t>
+  </si>
+  <si>
+    <t>Generate or update the documentation for your package</t>
+  </si>
+  <si>
+    <t>usethis</t>
+  </si>
+  <si>
+    <t>create_package</t>
+  </si>
+  <si>
+    <t>use_mit_license</t>
+  </si>
+  <si>
+    <t>use_package</t>
+  </si>
+  <si>
+    <t>use_r</t>
+  </si>
+  <si>
+    <t>Create an R package</t>
+  </si>
+  <si>
+    <t>Specify the MIT license to describe package usage rights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a script for a package function </t>
+  </si>
+  <si>
+    <t>Load all of the functions assigned to a package</t>
+  </si>
+  <si>
+    <t>Test a package for errors</t>
+  </si>
+  <si>
+    <t>Add a dependency on another package</t>
+  </si>
+  <si>
+    <t>Install a custom package and its dependencies</t>
   </si>
 </sst>
 </file>
@@ -2998,10 +3052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26B7B1B-D76F-6446-A51A-BD765778C143}">
-  <dimension ref="A1:D330"/>
+  <dimension ref="A1:D338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A314" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D325" sqref="D325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4343,58 +4397,58 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>82</v>
+        <v>706</v>
       </c>
       <c r="B96" t="s">
-        <v>228</v>
+        <v>708</v>
       </c>
       <c r="C96" t="s">
         <v>418</v>
       </c>
       <c r="D96" t="s">
-        <v>229</v>
+        <v>721</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>82</v>
+        <v>706</v>
       </c>
       <c r="B97" t="s">
-        <v>230</v>
+        <v>707</v>
       </c>
       <c r="C97" t="s">
         <v>418</v>
       </c>
       <c r="D97" t="s">
-        <v>231</v>
+        <v>711</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>82</v>
+        <v>706</v>
       </c>
       <c r="B98" t="s">
-        <v>83</v>
+        <v>709</v>
       </c>
       <c r="C98" t="s">
         <v>418</v>
       </c>
       <c r="D98" t="s">
-        <v>84</v>
+        <v>723</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>82</v>
+        <v>706</v>
       </c>
       <c r="B99" t="s">
-        <v>232</v>
+        <v>710</v>
       </c>
       <c r="C99" t="s">
         <v>418</v>
       </c>
       <c r="D99" t="s">
-        <v>233</v>
+        <v>720</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -4402,13 +4456,13 @@
         <v>82</v>
       </c>
       <c r="B100" t="s">
-        <v>85</v>
+        <v>228</v>
       </c>
       <c r="C100" t="s">
         <v>418</v>
       </c>
       <c r="D100" t="s">
-        <v>86</v>
+        <v>229</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -4416,13 +4470,13 @@
         <v>82</v>
       </c>
       <c r="B101" t="s">
-        <v>576</v>
+        <v>230</v>
       </c>
       <c r="C101" t="s">
         <v>418</v>
       </c>
       <c r="D101" t="s">
-        <v>577</v>
+        <v>231</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -4430,13 +4484,13 @@
         <v>82</v>
       </c>
       <c r="B102" t="s">
-        <v>691</v>
+        <v>83</v>
       </c>
       <c r="C102" t="s">
         <v>418</v>
       </c>
       <c r="D102" t="s">
-        <v>692</v>
+        <v>84</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -4444,13 +4498,13 @@
         <v>82</v>
       </c>
       <c r="B103" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C103" t="s">
         <v>418</v>
       </c>
       <c r="D103" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -4458,13 +4512,13 @@
         <v>82</v>
       </c>
       <c r="B104" t="s">
-        <v>236</v>
+        <v>85</v>
       </c>
       <c r="C104" t="s">
         <v>418</v>
       </c>
       <c r="D104" t="s">
-        <v>237</v>
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -4472,13 +4526,13 @@
         <v>82</v>
       </c>
       <c r="B105" t="s">
-        <v>87</v>
+        <v>576</v>
       </c>
       <c r="C105" t="s">
         <v>418</v>
       </c>
       <c r="D105" t="s">
-        <v>88</v>
+        <v>577</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -4486,13 +4540,13 @@
         <v>82</v>
       </c>
       <c r="B106" t="s">
-        <v>89</v>
+        <v>691</v>
       </c>
       <c r="C106" t="s">
         <v>418</v>
       </c>
       <c r="D106" t="s">
-        <v>90</v>
+        <v>692</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -4500,27 +4554,27 @@
         <v>82</v>
       </c>
       <c r="B107" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C107" t="s">
         <v>418</v>
       </c>
       <c r="D107" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>236</v>
       </c>
       <c r="C108" t="s">
         <v>418</v>
       </c>
       <c r="D108" t="s">
-        <v>125</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -4528,13 +4582,13 @@
         <v>82</v>
       </c>
       <c r="B109" t="s">
-        <v>240</v>
+        <v>87</v>
       </c>
       <c r="C109" t="s">
         <v>418</v>
       </c>
       <c r="D109" t="s">
-        <v>241</v>
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -4542,13 +4596,13 @@
         <v>82</v>
       </c>
       <c r="B110" t="s">
-        <v>242</v>
+        <v>89</v>
       </c>
       <c r="C110" t="s">
         <v>418</v>
       </c>
       <c r="D110" t="s">
-        <v>243</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -4556,27 +4610,27 @@
         <v>82</v>
       </c>
       <c r="B111" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C111" t="s">
         <v>418</v>
       </c>
       <c r="D111" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="B112" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="C112" t="s">
         <v>418</v>
       </c>
       <c r="D112" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -4584,13 +4638,13 @@
         <v>82</v>
       </c>
       <c r="B113" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C113" t="s">
         <v>418</v>
       </c>
       <c r="D113" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -4598,13 +4652,13 @@
         <v>82</v>
       </c>
       <c r="B114" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C114" t="s">
         <v>418</v>
       </c>
       <c r="D114" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -4612,13 +4666,13 @@
         <v>82</v>
       </c>
       <c r="B115" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C115" t="s">
         <v>418</v>
       </c>
       <c r="D115" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -4626,13 +4680,13 @@
         <v>82</v>
       </c>
       <c r="B116" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C116" t="s">
         <v>418</v>
       </c>
       <c r="D116" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -4640,13 +4694,13 @@
         <v>82</v>
       </c>
       <c r="B117" t="s">
-        <v>95</v>
+        <v>246</v>
       </c>
       <c r="C117" t="s">
         <v>418</v>
       </c>
       <c r="D117" t="s">
-        <v>96</v>
+        <v>247</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -4654,13 +4708,13 @@
         <v>82</v>
       </c>
       <c r="B118" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C118" t="s">
         <v>418</v>
       </c>
       <c r="D118" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -4668,13 +4722,13 @@
         <v>82</v>
       </c>
       <c r="B119" t="s">
-        <v>97</v>
+        <v>250</v>
       </c>
       <c r="C119" t="s">
         <v>418</v>
       </c>
       <c r="D119" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -4682,13 +4736,13 @@
         <v>82</v>
       </c>
       <c r="B120" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C120" t="s">
         <v>418</v>
       </c>
       <c r="D120" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -4696,13 +4750,13 @@
         <v>82</v>
       </c>
       <c r="B121" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C121" t="s">
         <v>418</v>
       </c>
       <c r="D121" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -4710,13 +4764,13 @@
         <v>82</v>
       </c>
       <c r="B122" t="s">
-        <v>103</v>
+        <v>252</v>
       </c>
       <c r="C122" t="s">
         <v>418</v>
       </c>
       <c r="D122" t="s">
-        <v>416</v>
+        <v>253</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -4724,13 +4778,13 @@
         <v>82</v>
       </c>
       <c r="B123" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C123" t="s">
         <v>418</v>
       </c>
       <c r="D123" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -4738,13 +4792,13 @@
         <v>82</v>
       </c>
       <c r="B124" t="s">
-        <v>686</v>
+        <v>99</v>
       </c>
       <c r="C124" t="s">
         <v>418</v>
       </c>
       <c r="D124" t="s">
-        <v>687</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -4752,13 +4806,13 @@
         <v>82</v>
       </c>
       <c r="B125" t="s">
-        <v>254</v>
+        <v>101</v>
       </c>
       <c r="C125" t="s">
         <v>418</v>
       </c>
       <c r="D125" t="s">
-        <v>255</v>
+        <v>102</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -4766,13 +4820,13 @@
         <v>82</v>
       </c>
       <c r="B126" t="s">
-        <v>256</v>
+        <v>103</v>
       </c>
       <c r="C126" t="s">
         <v>418</v>
       </c>
       <c r="D126" t="s">
-        <v>257</v>
+        <v>416</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -4780,13 +4834,13 @@
         <v>82</v>
       </c>
       <c r="B127" t="s">
-        <v>258</v>
+        <v>104</v>
       </c>
       <c r="C127" t="s">
         <v>418</v>
       </c>
       <c r="D127" t="s">
-        <v>259</v>
+        <v>105</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -4794,13 +4848,13 @@
         <v>82</v>
       </c>
       <c r="B128" t="s">
-        <v>260</v>
+        <v>686</v>
       </c>
       <c r="C128" t="s">
         <v>418</v>
       </c>
       <c r="D128" t="s">
-        <v>261</v>
+        <v>687</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -4808,13 +4862,13 @@
         <v>82</v>
       </c>
       <c r="B129" t="s">
-        <v>106</v>
+        <v>254</v>
       </c>
       <c r="C129" t="s">
         <v>418</v>
       </c>
       <c r="D129" t="s">
-        <v>107</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -4822,27 +4876,27 @@
         <v>82</v>
       </c>
       <c r="B130" t="s">
-        <v>108</v>
+        <v>256</v>
       </c>
       <c r="C130" t="s">
         <v>418</v>
       </c>
       <c r="D130" t="s">
-        <v>109</v>
+        <v>257</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>683</v>
+        <v>82</v>
       </c>
       <c r="B131" t="s">
-        <v>684</v>
+        <v>258</v>
       </c>
       <c r="C131" t="s">
         <v>418</v>
       </c>
       <c r="D131" t="s">
-        <v>685</v>
+        <v>259</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -4850,13 +4904,13 @@
         <v>82</v>
       </c>
       <c r="B132" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C132" t="s">
         <v>418</v>
       </c>
       <c r="D132" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -4864,83 +4918,83 @@
         <v>82</v>
       </c>
       <c r="B133" t="s">
-        <v>264</v>
+        <v>106</v>
       </c>
       <c r="C133" t="s">
         <v>418</v>
       </c>
       <c r="D133" t="s">
-        <v>265</v>
+        <v>107</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>700</v>
+        <v>82</v>
       </c>
       <c r="B134" t="s">
-        <v>701</v>
+        <v>108</v>
       </c>
       <c r="C134" t="s">
         <v>418</v>
       </c>
       <c r="D134" t="s">
-        <v>702</v>
+        <v>109</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>266</v>
+        <v>683</v>
       </c>
       <c r="B135" t="s">
-        <v>267</v>
+        <v>684</v>
       </c>
       <c r="C135" t="s">
         <v>418</v>
       </c>
       <c r="D135" t="s">
-        <v>268</v>
+        <v>685</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>266</v>
+        <v>82</v>
       </c>
       <c r="B136" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C136" t="s">
         <v>418</v>
       </c>
       <c r="D136" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>266</v>
+        <v>82</v>
       </c>
       <c r="B137" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C137" t="s">
         <v>418</v>
       </c>
       <c r="D137" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>266</v>
+        <v>700</v>
       </c>
       <c r="B138" t="s">
-        <v>273</v>
+        <v>701</v>
       </c>
       <c r="C138" t="s">
         <v>418</v>
       </c>
       <c r="D138" t="s">
-        <v>274</v>
+        <v>702</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -4948,69 +5002,69 @@
         <v>266</v>
       </c>
       <c r="B139" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C139" t="s">
         <v>418</v>
       </c>
       <c r="D139" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B140" t="s">
-        <v>10</v>
+        <v>269</v>
       </c>
       <c r="C140" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D140" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B141" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C141" t="s">
         <v>418</v>
       </c>
       <c r="D141" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B142" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C142" t="s">
         <v>418</v>
       </c>
       <c r="D142" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B143" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C143" t="s">
         <v>418</v>
       </c>
       <c r="D143" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -5018,13 +5072,13 @@
         <v>277</v>
       </c>
       <c r="B144" t="s">
-        <v>285</v>
+        <v>10</v>
       </c>
       <c r="C144" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D144" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -5032,13 +5086,13 @@
         <v>277</v>
       </c>
       <c r="B145" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C145" t="s">
         <v>418</v>
       </c>
       <c r="D145" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -5046,13 +5100,13 @@
         <v>277</v>
       </c>
       <c r="B146" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C146" t="s">
         <v>418</v>
       </c>
       <c r="D146" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -5060,13 +5114,13 @@
         <v>277</v>
       </c>
       <c r="B147" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C147" t="s">
         <v>418</v>
       </c>
       <c r="D147" t="s">
-        <v>663</v>
+        <v>284</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -5074,13 +5128,13 @@
         <v>277</v>
       </c>
       <c r="B148" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="C148" t="s">
         <v>418</v>
       </c>
       <c r="D148" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -5088,13 +5142,13 @@
         <v>277</v>
       </c>
       <c r="B149" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C149" t="s">
         <v>418</v>
       </c>
       <c r="D149" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -5102,13 +5156,13 @@
         <v>277</v>
       </c>
       <c r="B150" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C150" t="s">
         <v>418</v>
       </c>
       <c r="D150" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -5116,13 +5170,13 @@
         <v>277</v>
       </c>
       <c r="B151" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="C151" t="s">
         <v>418</v>
       </c>
       <c r="D151" t="s">
-        <v>299</v>
+        <v>663</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -5130,13 +5184,13 @@
         <v>277</v>
       </c>
       <c r="B152" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C152" t="s">
         <v>418</v>
       </c>
       <c r="D152" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -5144,13 +5198,13 @@
         <v>277</v>
       </c>
       <c r="B153" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C153" t="s">
         <v>418</v>
       </c>
       <c r="D153" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -5158,13 +5212,13 @@
         <v>277</v>
       </c>
       <c r="B154" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C154" t="s">
         <v>418</v>
       </c>
       <c r="D154" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -5172,13 +5226,13 @@
         <v>277</v>
       </c>
       <c r="B155" t="s">
-        <v>447</v>
+        <v>298</v>
       </c>
       <c r="C155" t="s">
         <v>418</v>
       </c>
       <c r="D155" t="s">
-        <v>448</v>
+        <v>299</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -5186,13 +5240,13 @@
         <v>277</v>
       </c>
       <c r="B156" t="s">
-        <v>459</v>
+        <v>300</v>
       </c>
       <c r="C156" t="s">
         <v>418</v>
       </c>
       <c r="D156" t="s">
-        <v>460</v>
+        <v>301</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -5200,13 +5254,13 @@
         <v>277</v>
       </c>
       <c r="B157" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C157" t="s">
         <v>418</v>
       </c>
       <c r="D157" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -5214,13 +5268,13 @@
         <v>277</v>
       </c>
       <c r="B158" t="s">
-        <v>446</v>
+        <v>304</v>
       </c>
       <c r="C158" t="s">
         <v>418</v>
       </c>
       <c r="D158" t="s">
-        <v>461</v>
+        <v>305</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -5228,13 +5282,13 @@
         <v>277</v>
       </c>
       <c r="B159" t="s">
-        <v>308</v>
+        <v>447</v>
       </c>
       <c r="C159" t="s">
         <v>418</v>
       </c>
       <c r="D159" t="s">
-        <v>309</v>
+        <v>448</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -5242,13 +5296,13 @@
         <v>277</v>
       </c>
       <c r="B160" t="s">
-        <v>310</v>
+        <v>459</v>
       </c>
       <c r="C160" t="s">
         <v>418</v>
       </c>
       <c r="D160" t="s">
-        <v>311</v>
+        <v>460</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -5256,13 +5310,13 @@
         <v>277</v>
       </c>
       <c r="B161" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C161" t="s">
         <v>418</v>
       </c>
       <c r="D161" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -5270,13 +5324,13 @@
         <v>277</v>
       </c>
       <c r="B162" t="s">
-        <v>314</v>
+        <v>446</v>
       </c>
       <c r="C162" t="s">
         <v>418</v>
       </c>
       <c r="D162" t="s">
-        <v>315</v>
+        <v>461</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -5284,13 +5338,13 @@
         <v>277</v>
       </c>
       <c r="B163" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C163" t="s">
         <v>418</v>
       </c>
       <c r="D163" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -5298,13 +5352,13 @@
         <v>277</v>
       </c>
       <c r="B164" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C164" t="s">
         <v>418</v>
       </c>
       <c r="D164" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -5312,13 +5366,13 @@
         <v>277</v>
       </c>
       <c r="B165" t="s">
-        <v>462</v>
+        <v>312</v>
       </c>
       <c r="C165" t="s">
         <v>418</v>
       </c>
       <c r="D165" t="s">
-        <v>463</v>
+        <v>313</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -5326,13 +5380,13 @@
         <v>277</v>
       </c>
       <c r="B166" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C166" t="s">
         <v>418</v>
       </c>
       <c r="D166" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -5340,13 +5394,13 @@
         <v>277</v>
       </c>
       <c r="B167" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C167" t="s">
         <v>418</v>
       </c>
       <c r="D167" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -5354,13 +5408,13 @@
         <v>277</v>
       </c>
       <c r="B168" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C168" t="s">
         <v>418</v>
       </c>
       <c r="D168" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -5368,13 +5422,13 @@
         <v>277</v>
       </c>
       <c r="B169" t="s">
-        <v>326</v>
+        <v>462</v>
       </c>
       <c r="C169" t="s">
         <v>418</v>
       </c>
       <c r="D169" t="s">
-        <v>327</v>
+        <v>463</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -5382,13 +5436,13 @@
         <v>277</v>
       </c>
       <c r="B170" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C170" t="s">
         <v>418</v>
       </c>
       <c r="D170" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -5396,13 +5450,13 @@
         <v>277</v>
       </c>
       <c r="B171" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="C171" t="s">
         <v>418</v>
       </c>
       <c r="D171" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -5410,13 +5464,13 @@
         <v>277</v>
       </c>
       <c r="B172" t="s">
-        <v>442</v>
+        <v>324</v>
       </c>
       <c r="C172" t="s">
         <v>418</v>
       </c>
       <c r="D172" t="s">
-        <v>443</v>
+        <v>325</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -5424,209 +5478,209 @@
         <v>277</v>
       </c>
       <c r="B173" t="s">
-        <v>445</v>
+        <v>326</v>
       </c>
       <c r="C173" t="s">
         <v>418</v>
       </c>
       <c r="D173" t="s">
-        <v>444</v>
+        <v>327</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>597</v>
+        <v>277</v>
       </c>
       <c r="B174" t="s">
-        <v>598</v>
+        <v>328</v>
       </c>
       <c r="C174" t="s">
         <v>418</v>
       </c>
       <c r="D174" t="s">
-        <v>599</v>
+        <v>329</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>611</v>
+        <v>277</v>
       </c>
       <c r="B175" t="s">
-        <v>612</v>
+        <v>330</v>
       </c>
       <c r="C175" t="s">
         <v>418</v>
       </c>
       <c r="D175" t="s">
-        <v>640</v>
+        <v>331</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>611</v>
+        <v>277</v>
       </c>
       <c r="B176" t="s">
-        <v>633</v>
+        <v>442</v>
       </c>
       <c r="C176" t="s">
         <v>418</v>
       </c>
       <c r="D176" t="s">
-        <v>641</v>
+        <v>443</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>609</v>
+        <v>277</v>
       </c>
       <c r="B177" t="s">
-        <v>610</v>
+        <v>445</v>
       </c>
       <c r="C177" t="s">
         <v>418</v>
       </c>
       <c r="D177" t="s">
-        <v>642</v>
+        <v>444</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>609</v>
+        <v>597</v>
       </c>
       <c r="B178" t="s">
-        <v>634</v>
+        <v>598</v>
       </c>
       <c r="C178" t="s">
         <v>418</v>
       </c>
       <c r="D178" t="s">
-        <v>656</v>
+        <v>599</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B179" t="s">
-        <v>635</v>
+        <v>612</v>
       </c>
       <c r="C179" t="s">
         <v>418</v>
       </c>
       <c r="D179" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>332</v>
+        <v>611</v>
       </c>
       <c r="B180" t="s">
-        <v>333</v>
+        <v>633</v>
       </c>
       <c r="C180" t="s">
         <v>418</v>
       </c>
       <c r="D180" t="s">
-        <v>334</v>
+        <v>641</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>332</v>
+        <v>609</v>
       </c>
       <c r="B181" t="s">
-        <v>335</v>
+        <v>610</v>
       </c>
       <c r="C181" t="s">
         <v>418</v>
       </c>
       <c r="D181" t="s">
-        <v>336</v>
+        <v>642</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>110</v>
+        <v>609</v>
       </c>
       <c r="B182" t="s">
-        <v>111</v>
+        <v>634</v>
       </c>
       <c r="C182" t="s">
         <v>418</v>
       </c>
       <c r="D182" t="s">
-        <v>112</v>
+        <v>656</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>110</v>
+        <v>609</v>
       </c>
       <c r="B183" t="s">
-        <v>337</v>
+        <v>635</v>
       </c>
       <c r="C183" t="s">
         <v>418</v>
       </c>
       <c r="D183" t="s">
-        <v>338</v>
+        <v>643</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>113</v>
+        <v>332</v>
       </c>
       <c r="B184" t="s">
-        <v>114</v>
+        <v>333</v>
       </c>
       <c r="C184" t="s">
         <v>418</v>
       </c>
       <c r="D184" t="s">
-        <v>115</v>
+        <v>334</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>113</v>
+        <v>332</v>
       </c>
       <c r="B185" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C185" t="s">
         <v>418</v>
       </c>
       <c r="D185" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B186" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C186" t="s">
         <v>418</v>
       </c>
       <c r="D186" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B187" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C187" t="s">
         <v>418</v>
       </c>
       <c r="D187" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -5634,13 +5688,13 @@
         <v>113</v>
       </c>
       <c r="B188" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C188" t="s">
         <v>418</v>
       </c>
       <c r="D188" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -5648,13 +5702,13 @@
         <v>113</v>
       </c>
       <c r="B189" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C189" t="s">
         <v>418</v>
       </c>
       <c r="D189" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -5662,13 +5716,13 @@
         <v>113</v>
       </c>
       <c r="B190" t="s">
-        <v>345</v>
+        <v>116</v>
       </c>
       <c r="C190" t="s">
         <v>418</v>
       </c>
       <c r="D190" t="s">
-        <v>346</v>
+        <v>117</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -5676,13 +5730,13 @@
         <v>113</v>
       </c>
       <c r="B191" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C191" t="s">
         <v>418</v>
       </c>
       <c r="D191" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
@@ -5690,125 +5744,125 @@
         <v>113</v>
       </c>
       <c r="B192" t="s">
-        <v>347</v>
+        <v>118</v>
       </c>
       <c r="C192" t="s">
         <v>418</v>
       </c>
       <c r="D192" t="s">
-        <v>348</v>
+        <v>119</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B193" t="s">
-        <v>121</v>
+        <v>343</v>
       </c>
       <c r="C193" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D193" t="s">
-        <v>122</v>
+        <v>344</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B194" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C194" t="s">
         <v>418</v>
       </c>
       <c r="D194" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>514</v>
+        <v>113</v>
       </c>
       <c r="B195" t="s">
-        <v>515</v>
+        <v>349</v>
       </c>
       <c r="C195" t="s">
         <v>418</v>
       </c>
       <c r="D195" t="s">
-        <v>516</v>
+        <v>350</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>604</v>
+        <v>113</v>
       </c>
       <c r="B196" t="s">
-        <v>605</v>
+        <v>347</v>
       </c>
       <c r="C196" t="s">
         <v>418</v>
       </c>
       <c r="D196" t="s">
-        <v>644</v>
+        <v>348</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B197" t="s">
-        <v>353</v>
+        <v>121</v>
       </c>
       <c r="C197" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D197" t="s">
-        <v>354</v>
+        <v>122</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B198" t="s">
-        <v>127</v>
+        <v>351</v>
       </c>
       <c r="C198" t="s">
         <v>418</v>
       </c>
       <c r="D198" t="s">
-        <v>128</v>
+        <v>352</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>126</v>
+        <v>514</v>
       </c>
       <c r="B199" t="s">
-        <v>487</v>
+        <v>515</v>
       </c>
       <c r="C199" t="s">
         <v>418</v>
       </c>
       <c r="D199" t="s">
-        <v>492</v>
+        <v>516</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>126</v>
+        <v>604</v>
       </c>
       <c r="B200" t="s">
-        <v>486</v>
+        <v>605</v>
       </c>
       <c r="C200" t="s">
         <v>418</v>
       </c>
       <c r="D200" t="s">
-        <v>493</v>
+        <v>644</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -5816,13 +5870,13 @@
         <v>126</v>
       </c>
       <c r="B201" t="s">
-        <v>484</v>
+        <v>353</v>
       </c>
       <c r="C201" t="s">
         <v>418</v>
       </c>
       <c r="D201" t="s">
-        <v>494</v>
+        <v>354</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -5830,13 +5884,13 @@
         <v>126</v>
       </c>
       <c r="B202" t="s">
-        <v>485</v>
+        <v>127</v>
       </c>
       <c r="C202" t="s">
         <v>418</v>
       </c>
       <c r="D202" t="s">
-        <v>495</v>
+        <v>128</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
@@ -5844,13 +5898,13 @@
         <v>126</v>
       </c>
       <c r="B203" t="s">
-        <v>355</v>
+        <v>487</v>
       </c>
       <c r="C203" t="s">
         <v>418</v>
       </c>
       <c r="D203" t="s">
-        <v>356</v>
+        <v>492</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -5858,83 +5912,83 @@
         <v>126</v>
       </c>
       <c r="B204" t="s">
-        <v>129</v>
+        <v>486</v>
       </c>
       <c r="C204" t="s">
         <v>418</v>
       </c>
       <c r="D204" t="s">
-        <v>130</v>
+        <v>493</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>357</v>
+        <v>126</v>
       </c>
       <c r="B205" t="s">
-        <v>358</v>
+        <v>484</v>
       </c>
       <c r="C205" t="s">
         <v>418</v>
       </c>
       <c r="D205" t="s">
-        <v>359</v>
+        <v>494</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B206" t="s">
-        <v>132</v>
+        <v>485</v>
       </c>
       <c r="C206" t="s">
         <v>418</v>
       </c>
       <c r="D206" t="s">
-        <v>133</v>
+        <v>495</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B207" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C207" t="s">
         <v>418</v>
       </c>
       <c r="D207" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B208" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C208" t="s">
         <v>418</v>
       </c>
       <c r="D208" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>131</v>
+        <v>357</v>
       </c>
       <c r="B209" t="s">
-        <v>136</v>
+        <v>358</v>
       </c>
       <c r="C209" t="s">
         <v>418</v>
       </c>
       <c r="D209" t="s">
-        <v>137</v>
+        <v>359</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
@@ -5942,13 +5996,13 @@
         <v>131</v>
       </c>
       <c r="B210" t="s">
-        <v>362</v>
+        <v>132</v>
       </c>
       <c r="C210" t="s">
         <v>418</v>
       </c>
       <c r="D210" t="s">
-        <v>363</v>
+        <v>133</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -5956,153 +6010,153 @@
         <v>131</v>
       </c>
       <c r="B211" t="s">
-        <v>138</v>
+        <v>360</v>
       </c>
       <c r="C211" t="s">
         <v>418</v>
       </c>
       <c r="D211" t="s">
-        <v>575</v>
+        <v>361</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>364</v>
+        <v>131</v>
       </c>
       <c r="B212" t="s">
-        <v>365</v>
+        <v>134</v>
       </c>
       <c r="C212" t="s">
         <v>418</v>
       </c>
       <c r="D212" t="s">
-        <v>366</v>
+        <v>135</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>364</v>
+        <v>131</v>
       </c>
       <c r="B213" t="s">
-        <v>367</v>
+        <v>136</v>
       </c>
       <c r="C213" t="s">
         <v>418</v>
       </c>
       <c r="D213" t="s">
-        <v>368</v>
+        <v>137</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B214" t="s">
-        <v>142</v>
+        <v>362</v>
       </c>
       <c r="C214" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D214" t="s">
-        <v>143</v>
+        <v>363</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B215" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C215" t="s">
         <v>418</v>
       </c>
       <c r="D215" t="s">
-        <v>141</v>
+        <v>575</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>521</v>
+        <v>364</v>
       </c>
       <c r="B216" t="s">
-        <v>522</v>
+        <v>365</v>
       </c>
       <c r="C216" t="s">
         <v>418</v>
       </c>
       <c r="D216" t="s">
-        <v>523</v>
+        <v>366</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>676</v>
+        <v>364</v>
       </c>
       <c r="B217" t="s">
-        <v>677</v>
+        <v>367</v>
       </c>
       <c r="C217" t="s">
         <v>418</v>
       </c>
       <c r="D217" t="s">
-        <v>678</v>
+        <v>368</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>421</v>
+        <v>139</v>
       </c>
       <c r="B218" t="s">
-        <v>546</v>
+        <v>142</v>
       </c>
       <c r="C218" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D218" t="s">
-        <v>570</v>
+        <v>143</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>421</v>
+        <v>139</v>
       </c>
       <c r="B219" t="s">
-        <v>422</v>
+        <v>140</v>
       </c>
       <c r="C219" t="s">
         <v>418</v>
       </c>
       <c r="D219" t="s">
-        <v>432</v>
+        <v>141</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>421</v>
+        <v>521</v>
       </c>
       <c r="B220" t="s">
-        <v>506</v>
+        <v>522</v>
       </c>
       <c r="C220" t="s">
         <v>418</v>
       </c>
       <c r="D220" t="s">
-        <v>507</v>
+        <v>523</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>421</v>
+        <v>676</v>
       </c>
       <c r="B221" t="s">
-        <v>524</v>
+        <v>677</v>
       </c>
       <c r="C221" t="s">
         <v>418</v>
       </c>
       <c r="D221" t="s">
-        <v>525</v>
+        <v>678</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -6110,13 +6164,13 @@
         <v>421</v>
       </c>
       <c r="B222" t="s">
-        <v>423</v>
+        <v>546</v>
       </c>
       <c r="C222" t="s">
         <v>418</v>
       </c>
       <c r="D222" t="s">
-        <v>433</v>
+        <v>570</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -6124,13 +6178,13 @@
         <v>421</v>
       </c>
       <c r="B223" t="s">
-        <v>547</v>
+        <v>422</v>
       </c>
       <c r="C223" t="s">
         <v>418</v>
       </c>
       <c r="D223" t="s">
-        <v>569</v>
+        <v>432</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -6138,13 +6192,13 @@
         <v>421</v>
       </c>
       <c r="B224" t="s">
-        <v>424</v>
+        <v>506</v>
       </c>
       <c r="C224" t="s">
         <v>418</v>
       </c>
       <c r="D224" t="s">
-        <v>434</v>
+        <v>507</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -6152,13 +6206,13 @@
         <v>421</v>
       </c>
       <c r="B225" t="s">
-        <v>548</v>
+        <v>524</v>
       </c>
       <c r="C225" t="s">
         <v>418</v>
       </c>
       <c r="D225" t="s">
-        <v>568</v>
+        <v>525</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -6166,13 +6220,13 @@
         <v>421</v>
       </c>
       <c r="B226" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C226" t="s">
         <v>418</v>
       </c>
       <c r="D226" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -6180,13 +6234,13 @@
         <v>421</v>
       </c>
       <c r="B227" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C227" t="s">
         <v>418</v>
       </c>
       <c r="D227" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
@@ -6194,13 +6248,13 @@
         <v>421</v>
       </c>
       <c r="B228" t="s">
-        <v>453</v>
+        <v>424</v>
       </c>
       <c r="C228" t="s">
         <v>418</v>
       </c>
       <c r="D228" t="s">
-        <v>454</v>
+        <v>434</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
@@ -6208,13 +6262,13 @@
         <v>421</v>
       </c>
       <c r="B229" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="C229" t="s">
         <v>418</v>
       </c>
       <c r="D229" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -6222,13 +6276,13 @@
         <v>421</v>
       </c>
       <c r="B230" t="s">
-        <v>550</v>
+        <v>425</v>
       </c>
       <c r="C230" t="s">
         <v>418</v>
       </c>
       <c r="D230" t="s">
-        <v>567</v>
+        <v>435</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
@@ -6236,13 +6290,13 @@
         <v>421</v>
       </c>
       <c r="B231" t="s">
-        <v>510</v>
+        <v>549</v>
       </c>
       <c r="C231" t="s">
         <v>418</v>
       </c>
       <c r="D231" t="s">
-        <v>511</v>
+        <v>571</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -6250,13 +6304,13 @@
         <v>421</v>
       </c>
       <c r="B232" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="C232" t="s">
         <v>418</v>
       </c>
       <c r="D232" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
@@ -6264,13 +6318,13 @@
         <v>421</v>
       </c>
       <c r="B233" t="s">
-        <v>512</v>
+        <v>561</v>
       </c>
       <c r="C233" t="s">
         <v>418</v>
       </c>
       <c r="D233" t="s">
-        <v>513</v>
+        <v>572</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -6278,13 +6332,13 @@
         <v>421</v>
       </c>
       <c r="B234" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="C234" t="s">
         <v>418</v>
       </c>
       <c r="D234" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
@@ -6292,13 +6346,13 @@
         <v>421</v>
       </c>
       <c r="B235" t="s">
-        <v>468</v>
+        <v>510</v>
       </c>
       <c r="C235" t="s">
         <v>418</v>
       </c>
       <c r="D235" t="s">
-        <v>469</v>
+        <v>511</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
@@ -6306,13 +6360,13 @@
         <v>421</v>
       </c>
       <c r="B236" t="s">
-        <v>551</v>
+        <v>464</v>
       </c>
       <c r="C236" t="s">
         <v>418</v>
       </c>
       <c r="D236" t="s">
-        <v>566</v>
+        <v>467</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -6320,13 +6374,13 @@
         <v>421</v>
       </c>
       <c r="B237" t="s">
-        <v>465</v>
+        <v>512</v>
       </c>
       <c r="C237" t="s">
         <v>418</v>
       </c>
       <c r="D237" t="s">
-        <v>466</v>
+        <v>513</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
@@ -6334,13 +6388,13 @@
         <v>421</v>
       </c>
       <c r="B238" t="s">
-        <v>426</v>
+        <v>545</v>
       </c>
       <c r="C238" t="s">
         <v>418</v>
       </c>
       <c r="D238" t="s">
-        <v>436</v>
+        <v>573</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
@@ -6348,13 +6402,13 @@
         <v>421</v>
       </c>
       <c r="B239" t="s">
-        <v>552</v>
+        <v>468</v>
       </c>
       <c r="C239" t="s">
         <v>418</v>
       </c>
       <c r="D239" t="s">
-        <v>565</v>
+        <v>469</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
@@ -6362,13 +6416,13 @@
         <v>421</v>
       </c>
       <c r="B240" t="s">
-        <v>427</v>
+        <v>551</v>
       </c>
       <c r="C240" t="s">
         <v>418</v>
       </c>
       <c r="D240" t="s">
-        <v>437</v>
+        <v>566</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
@@ -6376,13 +6430,13 @@
         <v>421</v>
       </c>
       <c r="B241" t="s">
-        <v>428</v>
+        <v>465</v>
       </c>
       <c r="C241" t="s">
         <v>418</v>
       </c>
       <c r="D241" t="s">
-        <v>438</v>
+        <v>466</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -6390,13 +6444,13 @@
         <v>421</v>
       </c>
       <c r="B242" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C242" t="s">
         <v>418</v>
       </c>
       <c r="D242" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
@@ -6404,13 +6458,13 @@
         <v>421</v>
       </c>
       <c r="B243" t="s">
-        <v>630</v>
+        <v>552</v>
       </c>
       <c r="C243" t="s">
         <v>418</v>
       </c>
       <c r="D243" t="s">
-        <v>645</v>
+        <v>565</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
@@ -6418,13 +6472,13 @@
         <v>421</v>
       </c>
       <c r="B244" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C244" t="s">
         <v>418</v>
       </c>
       <c r="D244" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
@@ -6432,13 +6486,13 @@
         <v>421</v>
       </c>
       <c r="B245" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C245" t="s">
         <v>418</v>
       </c>
       <c r="D245" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
@@ -6446,13 +6500,13 @@
         <v>421</v>
       </c>
       <c r="B246" t="s">
-        <v>519</v>
+        <v>429</v>
       </c>
       <c r="C246" t="s">
         <v>418</v>
       </c>
       <c r="D246" t="s">
-        <v>520</v>
+        <v>439</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
@@ -6460,13 +6514,13 @@
         <v>421</v>
       </c>
       <c r="B247" t="s">
-        <v>451</v>
+        <v>630</v>
       </c>
       <c r="C247" t="s">
         <v>418</v>
       </c>
       <c r="D247" t="s">
-        <v>452</v>
+        <v>645</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
@@ -6474,13 +6528,13 @@
         <v>421</v>
       </c>
       <c r="B248" t="s">
-        <v>517</v>
+        <v>430</v>
       </c>
       <c r="C248" t="s">
         <v>418</v>
       </c>
       <c r="D248" t="s">
-        <v>518</v>
+        <v>440</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
@@ -6488,167 +6542,167 @@
         <v>421</v>
       </c>
       <c r="B249" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
       <c r="C249" t="s">
         <v>418</v>
       </c>
       <c r="D249" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>602</v>
+        <v>421</v>
       </c>
       <c r="B250" t="s">
-        <v>603</v>
+        <v>519</v>
       </c>
       <c r="C250" t="s">
         <v>418</v>
       </c>
       <c r="D250" t="s">
-        <v>646</v>
+        <v>520</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>602</v>
+        <v>421</v>
       </c>
       <c r="B251" t="s">
-        <v>623</v>
+        <v>451</v>
       </c>
       <c r="C251" t="s">
         <v>418</v>
       </c>
       <c r="D251" t="s">
-        <v>647</v>
+        <v>452</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>615</v>
+        <v>421</v>
       </c>
       <c r="B252" t="s">
-        <v>616</v>
+        <v>517</v>
       </c>
       <c r="C252" t="s">
         <v>418</v>
       </c>
       <c r="D252" t="s">
-        <v>648</v>
+        <v>518</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>615</v>
+        <v>421</v>
       </c>
       <c r="B253" t="s">
-        <v>619</v>
+        <v>455</v>
       </c>
       <c r="C253" t="s">
         <v>418</v>
       </c>
       <c r="D253" t="s">
-        <v>649</v>
+        <v>456</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>620</v>
+        <v>602</v>
       </c>
       <c r="B254" t="s">
-        <v>621</v>
+        <v>603</v>
       </c>
       <c r="C254" t="s">
         <v>418</v>
       </c>
       <c r="D254" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>620</v>
+        <v>602</v>
       </c>
       <c r="B255" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C255" t="s">
         <v>418</v>
       </c>
       <c r="D255" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
       <c r="B256" t="s">
-        <v>629</v>
+        <v>616</v>
       </c>
       <c r="C256" t="s">
         <v>418</v>
       </c>
       <c r="D256" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>369</v>
+        <v>615</v>
       </c>
       <c r="B257" t="s">
-        <v>606</v>
+        <v>619</v>
       </c>
       <c r="C257" t="s">
         <v>418</v>
       </c>
       <c r="D257" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>369</v>
+        <v>620</v>
       </c>
       <c r="B258" t="s">
-        <v>614</v>
+        <v>621</v>
       </c>
       <c r="C258" t="s">
         <v>418</v>
       </c>
       <c r="D258" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>369</v>
+        <v>620</v>
       </c>
       <c r="B259" t="s">
-        <v>370</v>
+        <v>622</v>
       </c>
       <c r="C259" t="s">
         <v>418</v>
       </c>
       <c r="D259" t="s">
-        <v>371</v>
+        <v>651</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>369</v>
+        <v>628</v>
       </c>
       <c r="B260" t="s">
-        <v>584</v>
+        <v>629</v>
       </c>
       <c r="C260" t="s">
         <v>418</v>
       </c>
       <c r="D260" t="s">
-        <v>585</v>
+        <v>652</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
@@ -6656,13 +6710,13 @@
         <v>369</v>
       </c>
       <c r="B261" t="s">
-        <v>624</v>
+        <v>606</v>
       </c>
       <c r="C261" t="s">
         <v>418</v>
       </c>
       <c r="D261" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
@@ -6670,13 +6724,13 @@
         <v>369</v>
       </c>
       <c r="B262" t="s">
-        <v>372</v>
+        <v>614</v>
       </c>
       <c r="C262" t="s">
         <v>418</v>
       </c>
       <c r="D262" t="s">
-        <v>373</v>
+        <v>654</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
@@ -6684,13 +6738,13 @@
         <v>369</v>
       </c>
       <c r="B263" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C263" t="s">
         <v>418</v>
       </c>
       <c r="D263" t="s">
-        <v>419</v>
+        <v>371</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
@@ -6698,13 +6752,13 @@
         <v>369</v>
       </c>
       <c r="B264" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="C264" t="s">
         <v>418</v>
       </c>
       <c r="D264" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
@@ -6712,83 +6766,83 @@
         <v>369</v>
       </c>
       <c r="B265" t="s">
-        <v>375</v>
+        <v>624</v>
       </c>
       <c r="C265" t="s">
         <v>418</v>
       </c>
       <c r="D265" t="s">
-        <v>376</v>
+        <v>655</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>668</v>
+        <v>369</v>
       </c>
       <c r="B266" t="s">
-        <v>669</v>
+        <v>372</v>
       </c>
       <c r="C266" t="s">
         <v>418</v>
       </c>
       <c r="D266" t="s">
-        <v>670</v>
+        <v>373</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>144</v>
+        <v>369</v>
       </c>
       <c r="B267" t="s">
-        <v>145</v>
+        <v>374</v>
       </c>
       <c r="C267" t="s">
         <v>418</v>
       </c>
       <c r="D267" t="s">
-        <v>146</v>
+        <v>419</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>144</v>
+        <v>369</v>
       </c>
       <c r="B268" t="s">
-        <v>377</v>
+        <v>588</v>
       </c>
       <c r="C268" t="s">
         <v>418</v>
       </c>
       <c r="D268" t="s">
-        <v>378</v>
+        <v>589</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>144</v>
+        <v>369</v>
       </c>
       <c r="B269" t="s">
-        <v>590</v>
+        <v>375</v>
       </c>
       <c r="C269" t="s">
         <v>418</v>
       </c>
       <c r="D269" t="s">
-        <v>591</v>
+        <v>376</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>144</v>
+        <v>668</v>
       </c>
       <c r="B270" t="s">
-        <v>379</v>
+        <v>669</v>
       </c>
       <c r="C270" t="s">
         <v>418</v>
       </c>
       <c r="D270" t="s">
-        <v>380</v>
+        <v>670</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
@@ -6796,13 +6850,13 @@
         <v>144</v>
       </c>
       <c r="B271" t="s">
-        <v>381</v>
+        <v>145</v>
       </c>
       <c r="C271" t="s">
         <v>418</v>
       </c>
       <c r="D271" t="s">
-        <v>382</v>
+        <v>146</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
@@ -6810,13 +6864,13 @@
         <v>144</v>
       </c>
       <c r="B272" t="s">
-        <v>592</v>
+        <v>377</v>
       </c>
       <c r="C272" t="s">
         <v>418</v>
       </c>
       <c r="D272" t="s">
-        <v>594</v>
+        <v>378</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
@@ -6824,69 +6878,69 @@
         <v>144</v>
       </c>
       <c r="B273" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C273" t="s">
         <v>418</v>
       </c>
       <c r="D273" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B274" t="s">
-        <v>600</v>
+        <v>379</v>
       </c>
       <c r="C274" t="s">
         <v>418</v>
       </c>
       <c r="D274" t="s">
-        <v>601</v>
+        <v>380</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B275" t="s">
-        <v>578</v>
+        <v>381</v>
       </c>
       <c r="C275" t="s">
         <v>418</v>
       </c>
       <c r="D275" t="s">
-        <v>579</v>
+        <v>382</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B276" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="C276" t="s">
         <v>418</v>
       </c>
       <c r="D276" t="s">
-        <v>581</v>
+        <v>594</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>530</v>
+        <v>144</v>
       </c>
       <c r="B277" t="s">
-        <v>531</v>
+        <v>593</v>
       </c>
       <c r="C277" t="s">
         <v>418</v>
       </c>
       <c r="D277" t="s">
-        <v>538</v>
+        <v>595</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
@@ -6894,13 +6948,13 @@
         <v>530</v>
       </c>
       <c r="B278" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="C278" t="s">
         <v>418</v>
       </c>
       <c r="D278" t="s">
-        <v>657</v>
+        <v>601</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
@@ -6908,13 +6962,13 @@
         <v>530</v>
       </c>
       <c r="B279" t="s">
-        <v>351</v>
+        <v>578</v>
       </c>
       <c r="C279" t="s">
         <v>418</v>
       </c>
       <c r="D279" t="s">
-        <v>596</v>
+        <v>579</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
@@ -6922,13 +6976,13 @@
         <v>530</v>
       </c>
       <c r="B280" t="s">
-        <v>532</v>
+        <v>580</v>
       </c>
       <c r="C280" t="s">
         <v>418</v>
       </c>
       <c r="D280" t="s">
-        <v>539</v>
+        <v>581</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
@@ -6936,13 +6990,13 @@
         <v>530</v>
       </c>
       <c r="B281" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C281" t="s">
         <v>418</v>
       </c>
       <c r="D281" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
@@ -6950,13 +7004,13 @@
         <v>530</v>
       </c>
       <c r="B282" t="s">
-        <v>534</v>
+        <v>608</v>
       </c>
       <c r="C282" t="s">
         <v>418</v>
       </c>
       <c r="D282" t="s">
-        <v>541</v>
+        <v>657</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
@@ -6964,13 +7018,13 @@
         <v>530</v>
       </c>
       <c r="B283" t="s">
-        <v>535</v>
+        <v>351</v>
       </c>
       <c r="C283" t="s">
         <v>418</v>
       </c>
       <c r="D283" t="s">
-        <v>542</v>
+        <v>596</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
@@ -6978,13 +7032,13 @@
         <v>530</v>
       </c>
       <c r="B284" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C284" t="s">
         <v>418</v>
       </c>
       <c r="D284" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
@@ -6992,13 +7046,13 @@
         <v>530</v>
       </c>
       <c r="B285" t="s">
-        <v>586</v>
+        <v>533</v>
       </c>
       <c r="C285" t="s">
         <v>418</v>
       </c>
       <c r="D285" t="s">
-        <v>587</v>
+        <v>540</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
@@ -7006,13 +7060,13 @@
         <v>530</v>
       </c>
       <c r="B286" t="s">
-        <v>625</v>
+        <v>534</v>
       </c>
       <c r="C286" t="s">
         <v>418</v>
       </c>
       <c r="D286" t="s">
-        <v>658</v>
+        <v>541</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
@@ -7020,13 +7074,13 @@
         <v>530</v>
       </c>
       <c r="B287" t="s">
-        <v>626</v>
+        <v>535</v>
       </c>
       <c r="C287" t="s">
         <v>418</v>
       </c>
       <c r="D287" t="s">
-        <v>659</v>
+        <v>542</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
@@ -7034,13 +7088,13 @@
         <v>530</v>
       </c>
       <c r="B288" t="s">
-        <v>627</v>
+        <v>536</v>
       </c>
       <c r="C288" t="s">
         <v>418</v>
       </c>
       <c r="D288" t="s">
-        <v>660</v>
+        <v>543</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
@@ -7048,13 +7102,13 @@
         <v>530</v>
       </c>
       <c r="B289" t="s">
-        <v>632</v>
+        <v>586</v>
       </c>
       <c r="C289" t="s">
         <v>418</v>
       </c>
       <c r="D289" t="s">
-        <v>661</v>
+        <v>587</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
@@ -7062,125 +7116,125 @@
         <v>530</v>
       </c>
       <c r="B290" t="s">
-        <v>537</v>
+        <v>625</v>
       </c>
       <c r="C290" t="s">
         <v>418</v>
       </c>
       <c r="D290" t="s">
-        <v>544</v>
+        <v>658</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>147</v>
+        <v>530</v>
       </c>
       <c r="B291" t="s">
-        <v>457</v>
+        <v>626</v>
       </c>
       <c r="C291" t="s">
         <v>418</v>
       </c>
       <c r="D291" t="s">
-        <v>458</v>
+        <v>659</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>147</v>
+        <v>530</v>
       </c>
       <c r="B292" t="s">
-        <v>383</v>
+        <v>627</v>
       </c>
       <c r="C292" t="s">
         <v>418</v>
       </c>
       <c r="D292" t="s">
-        <v>384</v>
+        <v>660</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>147</v>
+        <v>530</v>
       </c>
       <c r="B293" t="s">
-        <v>147</v>
+        <v>632</v>
       </c>
       <c r="C293" t="s">
         <v>418</v>
       </c>
       <c r="D293" t="s">
-        <v>148</v>
+        <v>661</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>147</v>
+        <v>530</v>
       </c>
       <c r="B294" t="s">
-        <v>385</v>
+        <v>537</v>
       </c>
       <c r="C294" t="s">
         <v>418</v>
       </c>
       <c r="D294" t="s">
-        <v>386</v>
+        <v>544</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B295" t="s">
-        <v>387</v>
+        <v>457</v>
       </c>
       <c r="C295" t="s">
         <v>418</v>
       </c>
       <c r="D295" t="s">
-        <v>388</v>
+        <v>458</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B296" t="s">
-        <v>671</v>
+        <v>383</v>
       </c>
       <c r="C296" t="s">
         <v>418</v>
       </c>
       <c r="D296" t="s">
-        <v>672</v>
+        <v>384</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B297" t="s">
-        <v>664</v>
+        <v>147</v>
       </c>
       <c r="C297" t="s">
         <v>418</v>
       </c>
       <c r="D297" t="s">
-        <v>665</v>
+        <v>148</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B298" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C298" t="s">
         <v>418</v>
       </c>
       <c r="D298" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
@@ -7188,13 +7242,13 @@
         <v>149</v>
       </c>
       <c r="B299" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C299" t="s">
         <v>418</v>
       </c>
       <c r="D299" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
@@ -7202,13 +7256,13 @@
         <v>149</v>
       </c>
       <c r="B300" t="s">
-        <v>393</v>
+        <v>671</v>
       </c>
       <c r="C300" t="s">
         <v>418</v>
       </c>
       <c r="D300" t="s">
-        <v>394</v>
+        <v>672</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
@@ -7216,13 +7270,13 @@
         <v>149</v>
       </c>
       <c r="B301" t="s">
-        <v>395</v>
+        <v>664</v>
       </c>
       <c r="C301" t="s">
         <v>418</v>
       </c>
       <c r="D301" t="s">
-        <v>396</v>
+        <v>665</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
@@ -7230,13 +7284,13 @@
         <v>149</v>
       </c>
       <c r="B302" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C302" t="s">
         <v>418</v>
       </c>
       <c r="D302" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
@@ -7244,69 +7298,69 @@
         <v>149</v>
       </c>
       <c r="B303" t="s">
-        <v>666</v>
+        <v>391</v>
       </c>
       <c r="C303" t="s">
         <v>418</v>
       </c>
       <c r="D303" t="s">
-        <v>667</v>
+        <v>392</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>473</v>
+        <v>149</v>
       </c>
       <c r="B304" t="s">
-        <v>482</v>
+        <v>393</v>
       </c>
       <c r="C304" t="s">
         <v>418</v>
       </c>
       <c r="D304" t="s">
-        <v>496</v>
+        <v>394</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>473</v>
+        <v>149</v>
       </c>
       <c r="B305" t="s">
-        <v>526</v>
+        <v>395</v>
       </c>
       <c r="C305" t="s">
         <v>418</v>
       </c>
       <c r="D305" t="s">
-        <v>527</v>
+        <v>396</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>473</v>
+        <v>149</v>
       </c>
       <c r="B306" t="s">
-        <v>480</v>
+        <v>397</v>
       </c>
       <c r="C306" t="s">
         <v>418</v>
       </c>
       <c r="D306" t="s">
-        <v>497</v>
+        <v>398</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>473</v>
+        <v>149</v>
       </c>
       <c r="B307" t="s">
-        <v>481</v>
+        <v>666</v>
       </c>
       <c r="C307" t="s">
         <v>418</v>
       </c>
       <c r="D307" t="s">
-        <v>498</v>
+        <v>667</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
@@ -7314,13 +7368,13 @@
         <v>473</v>
       </c>
       <c r="B308" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="C308" t="s">
         <v>418</v>
       </c>
       <c r="D308" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
@@ -7328,13 +7382,13 @@
         <v>473</v>
       </c>
       <c r="B309" t="s">
-        <v>553</v>
+        <v>526</v>
       </c>
       <c r="C309" t="s">
         <v>418</v>
       </c>
       <c r="D309" t="s">
-        <v>562</v>
+        <v>527</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
@@ -7342,13 +7396,13 @@
         <v>473</v>
       </c>
       <c r="B310" t="s">
-        <v>504</v>
+        <v>480</v>
       </c>
       <c r="C310" t="s">
         <v>418</v>
       </c>
       <c r="D310" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
@@ -7356,13 +7410,13 @@
         <v>473</v>
       </c>
       <c r="B311" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C311" t="s">
         <v>418</v>
       </c>
       <c r="D311" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
@@ -7370,13 +7424,13 @@
         <v>473</v>
       </c>
       <c r="B312" t="s">
-        <v>508</v>
+        <v>476</v>
       </c>
       <c r="C312" t="s">
         <v>418</v>
       </c>
       <c r="D312" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
@@ -7384,13 +7438,13 @@
         <v>473</v>
       </c>
       <c r="B313" t="s">
-        <v>477</v>
+        <v>553</v>
       </c>
       <c r="C313" t="s">
         <v>418</v>
       </c>
       <c r="D313" t="s">
-        <v>501</v>
+        <v>562</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
@@ -7398,13 +7452,13 @@
         <v>473</v>
       </c>
       <c r="B314" t="s">
-        <v>474</v>
+        <v>504</v>
       </c>
       <c r="C314" t="s">
         <v>418</v>
       </c>
       <c r="D314" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
@@ -7412,222 +7466,334 @@
         <v>473</v>
       </c>
       <c r="B315" t="s">
-        <v>528</v>
+        <v>475</v>
       </c>
       <c r="C315" t="s">
         <v>418</v>
       </c>
       <c r="D315" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="B316" t="s">
-        <v>479</v>
+        <v>508</v>
       </c>
       <c r="C316" t="s">
         <v>418</v>
       </c>
       <c r="D316" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>399</v>
+        <v>473</v>
       </c>
       <c r="B317" t="s">
-        <v>400</v>
+        <v>477</v>
       </c>
       <c r="C317" t="s">
         <v>418</v>
       </c>
       <c r="D317" t="s">
-        <v>420</v>
+        <v>501</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>399</v>
+        <v>473</v>
       </c>
       <c r="B318" t="s">
-        <v>401</v>
+        <v>474</v>
       </c>
       <c r="C318" t="s">
         <v>418</v>
       </c>
       <c r="D318" t="s">
-        <v>402</v>
+        <v>502</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>399</v>
+        <v>473</v>
       </c>
       <c r="B319" t="s">
-        <v>403</v>
+        <v>528</v>
       </c>
       <c r="C319" t="s">
         <v>418</v>
       </c>
       <c r="D319" t="s">
-        <v>404</v>
+        <v>529</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>405</v>
+        <v>478</v>
       </c>
       <c r="B320" t="s">
-        <v>406</v>
+        <v>479</v>
       </c>
       <c r="C320" t="s">
         <v>418</v>
       </c>
       <c r="D320" t="s">
-        <v>407</v>
+        <v>503</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B321" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C321" t="s">
         <v>418</v>
       </c>
       <c r="D321" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>554</v>
+        <v>399</v>
       </c>
       <c r="B322" t="s">
-        <v>556</v>
+        <v>401</v>
       </c>
       <c r="C322" t="s">
         <v>418</v>
       </c>
       <c r="D322" t="s">
-        <v>563</v>
+        <v>402</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>554</v>
+        <v>399</v>
       </c>
       <c r="B323" t="s">
-        <v>555</v>
+        <v>403</v>
       </c>
       <c r="C323" t="s">
         <v>418</v>
       </c>
       <c r="D323" t="s">
-        <v>564</v>
+        <v>404</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>150</v>
+        <v>405</v>
       </c>
       <c r="B324" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C324" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D324" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>62</v>
+        <v>405</v>
       </c>
       <c r="B325" t="s">
-        <v>613</v>
+        <v>408</v>
       </c>
       <c r="C325" t="s">
         <v>418</v>
       </c>
       <c r="D325" t="s">
-        <v>637</v>
+        <v>409</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>150</v>
+        <v>554</v>
       </c>
       <c r="B326" t="s">
-        <v>151</v>
+        <v>556</v>
       </c>
       <c r="C326" t="s">
         <v>418</v>
       </c>
       <c r="D326" t="s">
-        <v>662</v>
+        <v>563</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>150</v>
+        <v>554</v>
       </c>
       <c r="B327" t="s">
-        <v>412</v>
+        <v>555</v>
       </c>
       <c r="C327" t="s">
         <v>418</v>
       </c>
       <c r="D327" t="s">
-        <v>413</v>
+        <v>564</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>150</v>
+        <v>712</v>
       </c>
       <c r="B328" t="s">
-        <v>557</v>
+        <v>713</v>
       </c>
       <c r="C328" t="s">
         <v>418</v>
       </c>
       <c r="D328" t="s">
-        <v>558</v>
+        <v>717</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>150</v>
+        <v>712</v>
       </c>
       <c r="B329" t="s">
-        <v>152</v>
+        <v>714</v>
       </c>
       <c r="C329" t="s">
         <v>418</v>
       </c>
       <c r="D329" t="s">
-        <v>153</v>
+        <v>718</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
+        <v>712</v>
+      </c>
+      <c r="B330" t="s">
+        <v>715</v>
+      </c>
+      <c r="C330" t="s">
+        <v>418</v>
+      </c>
+      <c r="D330" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>712</v>
+      </c>
+      <c r="B331" t="s">
+        <v>716</v>
+      </c>
+      <c r="C331" t="s">
+        <v>418</v>
+      </c>
+      <c r="D331" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
         <v>150</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B332" t="s">
+        <v>410</v>
+      </c>
+      <c r="C332" t="s">
+        <v>417</v>
+      </c>
+      <c r="D332" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>62</v>
+      </c>
+      <c r="B333" t="s">
+        <v>613</v>
+      </c>
+      <c r="C333" t="s">
+        <v>418</v>
+      </c>
+      <c r="D333" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>150</v>
+      </c>
+      <c r="B334" t="s">
+        <v>151</v>
+      </c>
+      <c r="C334" t="s">
+        <v>418</v>
+      </c>
+      <c r="D334" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A335" t="s">
+        <v>150</v>
+      </c>
+      <c r="B335" t="s">
+        <v>412</v>
+      </c>
+      <c r="C335" t="s">
+        <v>418</v>
+      </c>
+      <c r="D335" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A336" t="s">
+        <v>150</v>
+      </c>
+      <c r="B336" t="s">
+        <v>557</v>
+      </c>
+      <c r="C336" t="s">
+        <v>418</v>
+      </c>
+      <c r="D336" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>150</v>
+      </c>
+      <c r="B337" t="s">
+        <v>152</v>
+      </c>
+      <c r="C337" t="s">
+        <v>418</v>
+      </c>
+      <c r="D337" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
+        <v>150</v>
+      </c>
+      <c r="B338" t="s">
         <v>631</v>
       </c>
-      <c r="C330" t="s">
+      <c r="C338" t="s">
         <v>631</v>
       </c>
-      <c r="D330" t="s">
+      <c r="D338" t="s">
         <v>636</v>
       </c>
     </row>

</xml_diff>